<commit_message>
changed houers by 3D-Gehäuse zeichnen
</commit_message>
<xml_diff>
--- a/documentation/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
+++ b/documentation/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd4b8c2adf92642a/Berufsschule/BuP/5_Semester/Marvin/Zeitplan_Anforderungen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd4b8c2adf92642a/Berufsschule/BuP/5_Semester/Marvin/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="980" documentId="8_{E91F2863-CD3B-41DE-8D0C-65EAA4DE894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32BCF748-0C77-49C3-A9D7-3B823436B063}"/>
+  <xr:revisionPtr revIDLastSave="983" documentId="8_{E91F2863-CD3B-41DE-8D0C-65EAA4DE894C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05AAC655-C5EE-4BF7-817C-1B4BF1468115}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
   </bookViews>
@@ -986,7 +986,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1016,11 +1016,125 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1042,125 +1156,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1859,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730C7784-EAA3-4F75-A441-9364A27E8BAB}">
-  <dimension ref="A1:EL49"/>
+  <dimension ref="A1:EL46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="34" zoomScaleNormal="49" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="52" zoomScaleNormal="49" workbookViewId="0">
+      <selection activeCell="AL5" sqref="AL5:AR46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1871,823 +1866,823 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:142" ht="21">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
+      <c r="B1" s="66"/>
     </row>
     <row r="2" spans="1:142" ht="15" thickBot="1"/>
     <row r="3" spans="1:142" ht="15" thickBot="1">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="21">
         <f>SUM(C5:EL5,C7:EL7,C9:EL9,C11:EL11,C13:EL13,C15:EL15,C17:EL17,C19:EL19,C21:EL21,C23:EL23,C25:EL25,C27:EL27,C29:EL29,C31:EL31,C33:EL33)</f>
-        <v>107</v>
-      </c>
-      <c r="C3" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="73" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="73" t="s">
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="73" t="s">
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="74"/>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="74"/>
-      <c r="AB3" s="74"/>
-      <c r="AC3" s="74"/>
-      <c r="AD3" s="75"/>
-      <c r="AE3" s="73" t="s">
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="AF3" s="74"/>
-      <c r="AG3" s="74"/>
-      <c r="AH3" s="74"/>
-      <c r="AI3" s="74"/>
-      <c r="AJ3" s="74"/>
-      <c r="AK3" s="75"/>
-      <c r="AL3" s="73" t="s">
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="43"/>
+      <c r="AH3" s="43"/>
+      <c r="AI3" s="43"/>
+      <c r="AJ3" s="43"/>
+      <c r="AK3" s="44"/>
+      <c r="AL3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="AM3" s="74"/>
-      <c r="AN3" s="74"/>
-      <c r="AO3" s="74"/>
-      <c r="AP3" s="74"/>
-      <c r="AQ3" s="74"/>
-      <c r="AR3" s="75"/>
-      <c r="AS3" s="73" t="s">
+      <c r="AM3" s="43"/>
+      <c r="AN3" s="43"/>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="43"/>
+      <c r="AQ3" s="43"/>
+      <c r="AR3" s="44"/>
+      <c r="AS3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="AT3" s="74"/>
-      <c r="AU3" s="74"/>
-      <c r="AV3" s="74"/>
-      <c r="AW3" s="74"/>
-      <c r="AX3" s="74"/>
-      <c r="AY3" s="75"/>
-      <c r="AZ3" s="73" t="s">
+      <c r="AT3" s="43"/>
+      <c r="AU3" s="43"/>
+      <c r="AV3" s="43"/>
+      <c r="AW3" s="43"/>
+      <c r="AX3" s="43"/>
+      <c r="AY3" s="44"/>
+      <c r="AZ3" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="BA3" s="74"/>
-      <c r="BB3" s="74"/>
-      <c r="BC3" s="74"/>
-      <c r="BD3" s="74"/>
-      <c r="BE3" s="74"/>
-      <c r="BF3" s="75"/>
-      <c r="BG3" s="73" t="s">
+      <c r="BA3" s="43"/>
+      <c r="BB3" s="43"/>
+      <c r="BC3" s="43"/>
+      <c r="BD3" s="43"/>
+      <c r="BE3" s="43"/>
+      <c r="BF3" s="44"/>
+      <c r="BG3" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="BH3" s="74"/>
-      <c r="BI3" s="74"/>
-      <c r="BJ3" s="74"/>
-      <c r="BK3" s="74"/>
-      <c r="BL3" s="74"/>
-      <c r="BM3" s="75"/>
-      <c r="BN3" s="73" t="s">
+      <c r="BH3" s="43"/>
+      <c r="BI3" s="43"/>
+      <c r="BJ3" s="43"/>
+      <c r="BK3" s="43"/>
+      <c r="BL3" s="43"/>
+      <c r="BM3" s="44"/>
+      <c r="BN3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="BO3" s="74"/>
-      <c r="BP3" s="74"/>
-      <c r="BQ3" s="74"/>
-      <c r="BR3" s="74"/>
-      <c r="BS3" s="74"/>
-      <c r="BT3" s="75"/>
-      <c r="BU3" s="73" t="s">
+      <c r="BO3" s="43"/>
+      <c r="BP3" s="43"/>
+      <c r="BQ3" s="43"/>
+      <c r="BR3" s="43"/>
+      <c r="BS3" s="43"/>
+      <c r="BT3" s="44"/>
+      <c r="BU3" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="BV3" s="74"/>
-      <c r="BW3" s="74"/>
-      <c r="BX3" s="74"/>
-      <c r="BY3" s="74"/>
-      <c r="BZ3" s="74"/>
-      <c r="CA3" s="75"/>
-      <c r="CB3" s="73" t="s">
+      <c r="BV3" s="43"/>
+      <c r="BW3" s="43"/>
+      <c r="BX3" s="43"/>
+      <c r="BY3" s="43"/>
+      <c r="BZ3" s="43"/>
+      <c r="CA3" s="44"/>
+      <c r="CB3" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="CC3" s="74"/>
-      <c r="CD3" s="74"/>
-      <c r="CE3" s="74"/>
-      <c r="CF3" s="74"/>
-      <c r="CG3" s="74"/>
-      <c r="CH3" s="75"/>
-      <c r="CI3" s="73" t="s">
+      <c r="CC3" s="43"/>
+      <c r="CD3" s="43"/>
+      <c r="CE3" s="43"/>
+      <c r="CF3" s="43"/>
+      <c r="CG3" s="43"/>
+      <c r="CH3" s="44"/>
+      <c r="CI3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="CJ3" s="74"/>
-      <c r="CK3" s="74"/>
-      <c r="CL3" s="74"/>
-      <c r="CM3" s="74"/>
-      <c r="CN3" s="74"/>
-      <c r="CO3" s="75"/>
-      <c r="CP3" s="73" t="s">
+      <c r="CJ3" s="43"/>
+      <c r="CK3" s="43"/>
+      <c r="CL3" s="43"/>
+      <c r="CM3" s="43"/>
+      <c r="CN3" s="43"/>
+      <c r="CO3" s="44"/>
+      <c r="CP3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="CQ3" s="74"/>
-      <c r="CR3" s="74"/>
-      <c r="CS3" s="74"/>
-      <c r="CT3" s="74"/>
-      <c r="CU3" s="74"/>
-      <c r="CV3" s="75"/>
-      <c r="CW3" s="73" t="s">
+      <c r="CQ3" s="43"/>
+      <c r="CR3" s="43"/>
+      <c r="CS3" s="43"/>
+      <c r="CT3" s="43"/>
+      <c r="CU3" s="43"/>
+      <c r="CV3" s="44"/>
+      <c r="CW3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="CX3" s="74"/>
-      <c r="CY3" s="74"/>
-      <c r="CZ3" s="74"/>
-      <c r="DA3" s="74"/>
-      <c r="DB3" s="74"/>
-      <c r="DC3" s="75"/>
-      <c r="DD3" s="73" t="s">
+      <c r="CX3" s="43"/>
+      <c r="CY3" s="43"/>
+      <c r="CZ3" s="43"/>
+      <c r="DA3" s="43"/>
+      <c r="DB3" s="43"/>
+      <c r="DC3" s="44"/>
+      <c r="DD3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="DE3" s="74"/>
-      <c r="DF3" s="74"/>
-      <c r="DG3" s="74"/>
-      <c r="DH3" s="74"/>
-      <c r="DI3" s="74"/>
-      <c r="DJ3" s="75"/>
-      <c r="DK3" s="73" t="s">
+      <c r="DE3" s="43"/>
+      <c r="DF3" s="43"/>
+      <c r="DG3" s="43"/>
+      <c r="DH3" s="43"/>
+      <c r="DI3" s="43"/>
+      <c r="DJ3" s="44"/>
+      <c r="DK3" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="DL3" s="74"/>
-      <c r="DM3" s="74"/>
-      <c r="DN3" s="74"/>
-      <c r="DO3" s="74"/>
-      <c r="DP3" s="74"/>
-      <c r="DQ3" s="75"/>
-      <c r="DR3" s="73" t="s">
+      <c r="DL3" s="43"/>
+      <c r="DM3" s="43"/>
+      <c r="DN3" s="43"/>
+      <c r="DO3" s="43"/>
+      <c r="DP3" s="43"/>
+      <c r="DQ3" s="44"/>
+      <c r="DR3" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="DS3" s="74"/>
-      <c r="DT3" s="74"/>
-      <c r="DU3" s="74"/>
-      <c r="DV3" s="74"/>
-      <c r="DW3" s="74"/>
-      <c r="DX3" s="75"/>
-      <c r="DY3" s="76" t="s">
+      <c r="DS3" s="43"/>
+      <c r="DT3" s="43"/>
+      <c r="DU3" s="43"/>
+      <c r="DV3" s="43"/>
+      <c r="DW3" s="43"/>
+      <c r="DX3" s="44"/>
+      <c r="DY3" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="DZ3" s="77"/>
-      <c r="EA3" s="77"/>
-      <c r="EB3" s="77"/>
-      <c r="EC3" s="77"/>
-      <c r="ED3" s="77"/>
-      <c r="EE3" s="78"/>
-      <c r="EF3" s="76" t="s">
+      <c r="DZ3" s="46"/>
+      <c r="EA3" s="46"/>
+      <c r="EB3" s="46"/>
+      <c r="EC3" s="46"/>
+      <c r="ED3" s="46"/>
+      <c r="EE3" s="47"/>
+      <c r="EF3" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="EG3" s="77"/>
-      <c r="EH3" s="77"/>
-      <c r="EI3" s="77"/>
-      <c r="EJ3" s="77"/>
-      <c r="EK3" s="77"/>
-      <c r="EL3" s="78"/>
+      <c r="EG3" s="46"/>
+      <c r="EH3" s="46"/>
+      <c r="EI3" s="46"/>
+      <c r="EJ3" s="46"/>
+      <c r="EK3" s="46"/>
+      <c r="EL3" s="47"/>
     </row>
     <row r="4" spans="1:142" ht="15" thickBot="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="20">
         <f>SUM(C6:EL6,C8:EL8,C10:EL10,C12:EL12,C14:EL14,C16:EL16,C18:EL18,C20:EL20,C22:EL22,C24:EL24,C26:EL26,C28:EL28,C30:EL30,C32:EL32,C34:EL34)</f>
         <v>28</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="28" t="s">
+      <c r="N4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="28" t="s">
+      <c r="P4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="28" t="s">
+      <c r="R4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="28" t="s">
+      <c r="S4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="T4" s="28" t="s">
+      <c r="T4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="28" t="s">
+      <c r="U4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="28" t="s">
+      <c r="V4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="28" t="s">
+      <c r="W4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="28" t="s">
+      <c r="X4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="Y4" s="28" t="s">
+      <c r="Y4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Z4" s="28" t="s">
+      <c r="Z4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="28" t="s">
+      <c r="AA4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AB4" s="28" t="s">
+      <c r="AB4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AC4" s="28" t="s">
+      <c r="AC4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="28" t="s">
+      <c r="AD4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AE4" s="28" t="s">
+      <c r="AE4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AF4" s="28" t="s">
+      <c r="AF4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AG4" s="28" t="s">
+      <c r="AG4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AH4" s="28" t="s">
+      <c r="AH4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AI4" s="28" t="s">
+      <c r="AI4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AJ4" s="28" t="s">
+      <c r="AJ4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AK4" s="28" t="s">
+      <c r="AK4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AL4" s="28" t="s">
+      <c r="AL4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AM4" s="28" t="s">
+      <c r="AM4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AN4" s="28" t="s">
+      <c r="AN4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AO4" s="28" t="s">
+      <c r="AO4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AP4" s="28" t="s">
+      <c r="AP4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AQ4" s="28" t="s">
+      <c r="AQ4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AR4" s="28" t="s">
+      <c r="AR4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AS4" s="28" t="s">
+      <c r="AS4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AT4" s="28" t="s">
+      <c r="AT4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AU4" s="28" t="s">
+      <c r="AU4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AV4" s="28" t="s">
+      <c r="AV4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AW4" s="28" t="s">
+      <c r="AW4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AX4" s="28" t="s">
+      <c r="AX4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AY4" s="28" t="s">
+      <c r="AY4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AZ4" s="28" t="s">
+      <c r="AZ4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BA4" s="28" t="s">
+      <c r="BA4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="BB4" s="28" t="s">
+      <c r="BB4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="BC4" s="28" t="s">
+      <c r="BC4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="BD4" s="28" t="s">
+      <c r="BD4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BE4" s="28" t="s">
+      <c r="BE4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="BF4" s="28" t="s">
+      <c r="BF4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="BG4" s="28" t="s">
+      <c r="BG4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BH4" s="28" t="s">
+      <c r="BH4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="BI4" s="28" t="s">
+      <c r="BI4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="BJ4" s="28" t="s">
+      <c r="BJ4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="BK4" s="28" t="s">
+      <c r="BK4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BL4" s="28" t="s">
+      <c r="BL4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="BM4" s="28" t="s">
+      <c r="BM4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="BN4" s="28" t="s">
+      <c r="BN4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BO4" s="28" t="s">
+      <c r="BO4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="BP4" s="28" t="s">
+      <c r="BP4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="BQ4" s="28" t="s">
+      <c r="BQ4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="BR4" s="28" t="s">
+      <c r="BR4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BS4" s="28" t="s">
+      <c r="BS4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="BT4" s="28" t="s">
+      <c r="BT4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="BU4" s="28" t="s">
+      <c r="BU4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BV4" s="28" t="s">
+      <c r="BV4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="BW4" s="28" t="s">
+      <c r="BW4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="BX4" s="28" t="s">
+      <c r="BX4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="BY4" s="28" t="s">
+      <c r="BY4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="BZ4" s="28" t="s">
+      <c r="BZ4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="CA4" s="28" t="s">
+      <c r="CA4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CB4" s="28" t="s">
+      <c r="CB4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CC4" s="28" t="s">
+      <c r="CC4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="CD4" s="28" t="s">
+      <c r="CD4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="CE4" s="28" t="s">
+      <c r="CE4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="CF4" s="28" t="s">
+      <c r="CF4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="CG4" s="28" t="s">
+      <c r="CG4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="CH4" s="28" t="s">
+      <c r="CH4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CI4" s="28" t="s">
+      <c r="CI4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CJ4" s="28" t="s">
+      <c r="CJ4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="CK4" s="28" t="s">
+      <c r="CK4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="CL4" s="28" t="s">
+      <c r="CL4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="CM4" s="28" t="s">
+      <c r="CM4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="CN4" s="28" t="s">
+      <c r="CN4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="CO4" s="28" t="s">
+      <c r="CO4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CP4" s="28" t="s">
+      <c r="CP4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CQ4" s="28" t="s">
+      <c r="CQ4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="CR4" s="28" t="s">
+      <c r="CR4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="CS4" s="28" t="s">
+      <c r="CS4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="CT4" s="28" t="s">
+      <c r="CT4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="CU4" s="28" t="s">
+      <c r="CU4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="CV4" s="28" t="s">
+      <c r="CV4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CW4" s="28" t="s">
+      <c r="CW4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CX4" s="28" t="s">
+      <c r="CX4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="CY4" s="28" t="s">
+      <c r="CY4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="CZ4" s="28" t="s">
+      <c r="CZ4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="DA4" s="28" t="s">
+      <c r="DA4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="DB4" s="28" t="s">
+      <c r="DB4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="DC4" s="28" t="s">
+      <c r="DC4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="DD4" s="28" t="s">
+      <c r="DD4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="DE4" s="28" t="s">
+      <c r="DE4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="DF4" s="28" t="s">
+      <c r="DF4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="DG4" s="28" t="s">
+      <c r="DG4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="DH4" s="28" t="s">
+      <c r="DH4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="DI4" s="28" t="s">
+      <c r="DI4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="DJ4" s="28" t="s">
+      <c r="DJ4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="DK4" s="63" t="s">
+      <c r="DK4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="DL4" s="63" t="s">
+      <c r="DL4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="DM4" s="63" t="s">
+      <c r="DM4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="DN4" s="63" t="s">
+      <c r="DN4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="DO4" s="63" t="s">
+      <c r="DO4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="DP4" s="63" t="s">
+      <c r="DP4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="DQ4" s="63" t="s">
+      <c r="DQ4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="DR4" s="28" t="s">
+      <c r="DR4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="DS4" s="28" t="s">
+      <c r="DS4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="DT4" s="28" t="s">
+      <c r="DT4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="DU4" s="28" t="s">
+      <c r="DU4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="DV4" s="28" t="s">
+      <c r="DV4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="DW4" s="28" t="s">
+      <c r="DW4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="DX4" s="28" t="s">
+      <c r="DX4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="DY4" s="28" t="s">
+      <c r="DY4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="DZ4" s="28" t="s">
+      <c r="DZ4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="EA4" s="28" t="s">
+      <c r="EA4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="EB4" s="28" t="s">
+      <c r="EB4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="EC4" s="28" t="s">
+      <c r="EC4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="ED4" s="28" t="s">
+      <c r="ED4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="EE4" s="28" t="s">
+      <c r="EE4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="EF4" s="28" t="s">
+      <c r="EF4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="EG4" s="28" t="s">
+      <c r="EG4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="EH4" s="28" t="s">
+      <c r="EH4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="EI4" s="28" t="s">
+      <c r="EI4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="EJ4" s="28" t="s">
+      <c r="EJ4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="EK4" s="28" t="s">
+      <c r="EK4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="EL4" s="28" t="s">
+      <c r="EL4" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:142" ht="15" thickBot="1">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="33"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="43">
+      <c r="J5" s="22"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="27">
         <v>1</v>
       </c>
-      <c r="O5" s="33"/>
+      <c r="O5" s="23"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="43">
+      <c r="Q5" s="22"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="27">
         <v>1</v>
       </c>
-      <c r="V5" s="33"/>
+      <c r="V5" s="23"/>
       <c r="W5" s="7"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="33"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="43">
+      <c r="X5" s="22"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="27">
         <v>1</v>
       </c>
-      <c r="AC5" s="33"/>
+      <c r="AC5" s="23"/>
       <c r="AD5" s="7"/>
-      <c r="AE5" s="32"/>
-      <c r="AF5" s="33"/>
-      <c r="AG5" s="33"/>
-      <c r="AH5" s="33"/>
-      <c r="AI5" s="43">
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="27">
         <v>1</v>
       </c>
-      <c r="AJ5" s="33"/>
+      <c r="AJ5" s="23"/>
       <c r="AK5" s="7"/>
-      <c r="AL5" s="54" t="s">
+      <c r="AL5" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="AM5" s="55"/>
-      <c r="AN5" s="55"/>
-      <c r="AO5" s="55"/>
-      <c r="AP5" s="55"/>
-      <c r="AQ5" s="55"/>
-      <c r="AR5" s="56"/>
-      <c r="AS5" s="32"/>
-      <c r="AT5" s="33"/>
-      <c r="AU5" s="33"/>
-      <c r="AV5" s="33"/>
-      <c r="AW5" s="43">
+      <c r="AM5" s="50"/>
+      <c r="AN5" s="50"/>
+      <c r="AO5" s="50"/>
+      <c r="AP5" s="50"/>
+      <c r="AQ5" s="50"/>
+      <c r="AR5" s="51"/>
+      <c r="AS5" s="22"/>
+      <c r="AT5" s="23"/>
+      <c r="AU5" s="23"/>
+      <c r="AV5" s="23"/>
+      <c r="AW5" s="27">
         <v>1</v>
       </c>
-      <c r="AX5" s="33"/>
+      <c r="AX5" s="23"/>
       <c r="AY5" s="7"/>
-      <c r="AZ5" s="32"/>
-      <c r="BA5" s="33"/>
-      <c r="BB5" s="33"/>
-      <c r="BC5" s="33"/>
-      <c r="BD5" s="43">
+      <c r="AZ5" s="22"/>
+      <c r="BA5" s="23"/>
+      <c r="BB5" s="23"/>
+      <c r="BC5" s="23"/>
+      <c r="BD5" s="27">
         <v>1</v>
       </c>
-      <c r="BE5" s="33"/>
+      <c r="BE5" s="23"/>
       <c r="BF5" s="7"/>
-      <c r="BG5" s="32"/>
-      <c r="BH5" s="33"/>
-      <c r="BI5" s="33"/>
-      <c r="BJ5" s="33"/>
-      <c r="BK5" s="43">
+      <c r="BG5" s="22"/>
+      <c r="BH5" s="23"/>
+      <c r="BI5" s="23"/>
+      <c r="BJ5" s="23"/>
+      <c r="BK5" s="27">
         <v>1</v>
       </c>
-      <c r="BL5" s="33"/>
+      <c r="BL5" s="23"/>
       <c r="BM5" s="7"/>
-      <c r="BN5" s="32"/>
-      <c r="BO5" s="33"/>
-      <c r="BP5" s="33"/>
-      <c r="BQ5" s="33"/>
-      <c r="BR5" s="43">
+      <c r="BN5" s="22"/>
+      <c r="BO5" s="23"/>
+      <c r="BP5" s="23"/>
+      <c r="BQ5" s="23"/>
+      <c r="BR5" s="27">
         <v>1</v>
       </c>
-      <c r="BS5" s="33"/>
+      <c r="BS5" s="23"/>
       <c r="BT5" s="7"/>
-      <c r="BU5" s="32"/>
-      <c r="BV5" s="33"/>
-      <c r="BW5" s="33"/>
-      <c r="BX5" s="33"/>
-      <c r="BY5" s="43">
+      <c r="BU5" s="22"/>
+      <c r="BV5" s="23"/>
+      <c r="BW5" s="23"/>
+      <c r="BX5" s="23"/>
+      <c r="BY5" s="27">
         <v>1</v>
       </c>
-      <c r="BZ5" s="33"/>
+      <c r="BZ5" s="23"/>
       <c r="CA5" s="7"/>
-      <c r="CB5" s="32"/>
-      <c r="CC5" s="33"/>
-      <c r="CD5" s="33"/>
-      <c r="CE5" s="33"/>
-      <c r="CF5" s="43">
+      <c r="CB5" s="22"/>
+      <c r="CC5" s="23"/>
+      <c r="CD5" s="23"/>
+      <c r="CE5" s="23"/>
+      <c r="CF5" s="27">
         <v>1</v>
       </c>
-      <c r="CG5" s="33"/>
+      <c r="CG5" s="23"/>
       <c r="CH5" s="7"/>
-      <c r="CI5" s="32"/>
-      <c r="CJ5" s="33"/>
-      <c r="CK5" s="33"/>
-      <c r="CL5" s="33"/>
-      <c r="CM5" s="43">
+      <c r="CI5" s="22"/>
+      <c r="CJ5" s="23"/>
+      <c r="CK5" s="23"/>
+      <c r="CL5" s="23"/>
+      <c r="CM5" s="27">
         <v>1</v>
       </c>
-      <c r="CN5" s="33"/>
+      <c r="CN5" s="23"/>
       <c r="CO5" s="7"/>
-      <c r="CP5" s="32"/>
-      <c r="CQ5" s="33"/>
-      <c r="CR5" s="33"/>
-      <c r="CS5" s="33"/>
-      <c r="CT5" s="43">
+      <c r="CP5" s="22"/>
+      <c r="CQ5" s="23"/>
+      <c r="CR5" s="23"/>
+      <c r="CS5" s="23"/>
+      <c r="CT5" s="27">
         <v>1</v>
       </c>
-      <c r="CU5" s="33"/>
+      <c r="CU5" s="23"/>
       <c r="CV5" s="7"/>
-      <c r="CW5" s="32"/>
-      <c r="CX5" s="33"/>
-      <c r="CY5" s="33"/>
-      <c r="CZ5" s="33"/>
-      <c r="DA5" s="43">
+      <c r="CW5" s="22"/>
+      <c r="CX5" s="23"/>
+      <c r="CY5" s="23"/>
+      <c r="CZ5" s="23"/>
+      <c r="DA5" s="27">
         <v>1</v>
       </c>
-      <c r="DB5" s="33"/>
+      <c r="DB5" s="23"/>
       <c r="DC5" s="7"/>
-      <c r="DD5" s="32"/>
-      <c r="DE5" s="33"/>
-      <c r="DF5" s="33"/>
-      <c r="DG5" s="33"/>
-      <c r="DH5" s="43">
+      <c r="DD5" s="22"/>
+      <c r="DE5" s="23"/>
+      <c r="DF5" s="23"/>
+      <c r="DG5" s="23"/>
+      <c r="DH5" s="27">
         <v>1</v>
       </c>
-      <c r="DI5" s="33"/>
+      <c r="DI5" s="23"/>
       <c r="DJ5" s="7"/>
-      <c r="DK5" s="54" t="s">
+      <c r="DK5" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="DL5" s="46"/>
-      <c r="DM5" s="46"/>
-      <c r="DN5" s="46"/>
-      <c r="DO5" s="46"/>
-      <c r="DP5" s="46"/>
-      <c r="DQ5" s="47"/>
-      <c r="DR5" s="54" t="s">
+      <c r="DL5" s="58"/>
+      <c r="DM5" s="58"/>
+      <c r="DN5" s="58"/>
+      <c r="DO5" s="58"/>
+      <c r="DP5" s="58"/>
+      <c r="DQ5" s="59"/>
+      <c r="DR5" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="DS5" s="46"/>
-      <c r="DT5" s="46"/>
-      <c r="DU5" s="46"/>
-      <c r="DV5" s="46"/>
-      <c r="DW5" s="46"/>
-      <c r="DX5" s="47"/>
-      <c r="DY5" s="32"/>
-      <c r="DZ5" s="43">
+      <c r="DS5" s="58"/>
+      <c r="DT5" s="58"/>
+      <c r="DU5" s="58"/>
+      <c r="DV5" s="58"/>
+      <c r="DW5" s="58"/>
+      <c r="DX5" s="59"/>
+      <c r="DY5" s="22"/>
+      <c r="DZ5" s="27">
         <v>1</v>
       </c>
-      <c r="EA5" s="43">
+      <c r="EA5" s="27">
         <v>1</v>
       </c>
-      <c r="EB5" s="43">
+      <c r="EB5" s="27">
         <v>1</v>
       </c>
-      <c r="EC5" s="43">
+      <c r="EC5" s="27">
         <v>1</v>
       </c>
-      <c r="ED5" s="33"/>
+      <c r="ED5" s="23"/>
       <c r="EE5" s="7"/>
-      <c r="EF5" s="32"/>
-      <c r="EG5" s="33"/>
-      <c r="EH5" s="33"/>
-      <c r="EI5" s="33"/>
-      <c r="EJ5" s="33"/>
-      <c r="EK5" s="33"/>
+      <c r="EF5" s="22"/>
+      <c r="EG5" s="23"/>
+      <c r="EH5" s="23"/>
+      <c r="EI5" s="23"/>
+      <c r="EJ5" s="23"/>
+      <c r="EK5" s="23"/>
       <c r="EL5" s="7"/>
     </row>
     <row r="6" spans="1:142" ht="15" thickBot="1">
-      <c r="A6" s="67"/>
-      <c r="B6" s="36" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="2"/>
@@ -2701,7 +2696,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="64">
+      <c r="N6" s="31">
         <v>2</v>
       </c>
       <c r="O6" s="1"/>
@@ -2710,7 +2705,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
-      <c r="U6" s="64">
+      <c r="U6" s="31">
         <v>2</v>
       </c>
       <c r="V6" s="1"/>
@@ -2719,7 +2714,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AB6" s="64">
+      <c r="AB6" s="31">
         <v>2</v>
       </c>
       <c r="AC6" s="1"/>
@@ -2731,18 +2726,18 @@
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="3"/>
-      <c r="AL6" s="57"/>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="58"/>
-      <c r="AO6" s="58"/>
-      <c r="AP6" s="58"/>
-      <c r="AQ6" s="58"/>
-      <c r="AR6" s="59"/>
+      <c r="AL6" s="52"/>
+      <c r="AM6" s="53"/>
+      <c r="AN6" s="53"/>
+      <c r="AO6" s="53"/>
+      <c r="AP6" s="53"/>
+      <c r="AQ6" s="53"/>
+      <c r="AR6" s="54"/>
       <c r="AS6" s="2"/>
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
-      <c r="AW6" s="34"/>
+      <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
       <c r="AY6" s="3"/>
       <c r="AZ6" s="2"/>
@@ -2808,20 +2803,20 @@
       <c r="DH6" s="1"/>
       <c r="DI6" s="1"/>
       <c r="DJ6" s="3"/>
-      <c r="DK6" s="48"/>
-      <c r="DL6" s="49"/>
-      <c r="DM6" s="49"/>
-      <c r="DN6" s="49"/>
-      <c r="DO6" s="49"/>
-      <c r="DP6" s="49"/>
-      <c r="DQ6" s="50"/>
-      <c r="DR6" s="48"/>
-      <c r="DS6" s="49"/>
-      <c r="DT6" s="49"/>
-      <c r="DU6" s="49"/>
-      <c r="DV6" s="49"/>
-      <c r="DW6" s="49"/>
-      <c r="DX6" s="50"/>
+      <c r="DK6" s="60"/>
+      <c r="DL6" s="61"/>
+      <c r="DM6" s="61"/>
+      <c r="DN6" s="61"/>
+      <c r="DO6" s="61"/>
+      <c r="DP6" s="61"/>
+      <c r="DQ6" s="62"/>
+      <c r="DR6" s="60"/>
+      <c r="DS6" s="61"/>
+      <c r="DT6" s="61"/>
+      <c r="DU6" s="61"/>
+      <c r="DV6" s="61"/>
+      <c r="DW6" s="61"/>
+      <c r="DX6" s="62"/>
       <c r="DY6" s="2"/>
       <c r="DZ6" s="1"/>
       <c r="EA6" s="1"/>
@@ -2838,17 +2833,17 @@
       <c r="EL6" s="3"/>
     </row>
     <row r="7" spans="1:142" ht="15" thickBot="1">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="40">
+      <c r="D7" s="26">
         <v>2</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="26">
         <v>2</v>
       </c>
       <c r="F7" s="1"/>
@@ -2856,10 +2851,10 @@
       <c r="H7" s="1"/>
       <c r="I7" s="3"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="40">
+      <c r="K7" s="26">
         <v>2</v>
       </c>
-      <c r="L7" s="40">
+      <c r="L7" s="26">
         <v>2</v>
       </c>
       <c r="M7" s="1"/>
@@ -2882,18 +2877,18 @@
       <c r="AD7" s="3"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="1"/>
-      <c r="AG7" s="34"/>
+      <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="3"/>
-      <c r="AL7" s="57"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="58"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="59"/>
+      <c r="AL7" s="52"/>
+      <c r="AM7" s="53"/>
+      <c r="AN7" s="53"/>
+      <c r="AO7" s="53"/>
+      <c r="AP7" s="53"/>
+      <c r="AQ7" s="53"/>
+      <c r="AR7" s="54"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
@@ -2964,20 +2959,20 @@
       <c r="DH7" s="1"/>
       <c r="DI7" s="1"/>
       <c r="DJ7" s="3"/>
-      <c r="DK7" s="48"/>
-      <c r="DL7" s="49"/>
-      <c r="DM7" s="49"/>
-      <c r="DN7" s="49"/>
-      <c r="DO7" s="49"/>
-      <c r="DP7" s="49"/>
-      <c r="DQ7" s="50"/>
-      <c r="DR7" s="48"/>
-      <c r="DS7" s="49"/>
-      <c r="DT7" s="49"/>
-      <c r="DU7" s="49"/>
-      <c r="DV7" s="49"/>
-      <c r="DW7" s="49"/>
-      <c r="DX7" s="50"/>
+      <c r="DK7" s="60"/>
+      <c r="DL7" s="61"/>
+      <c r="DM7" s="61"/>
+      <c r="DN7" s="61"/>
+      <c r="DO7" s="61"/>
+      <c r="DP7" s="61"/>
+      <c r="DQ7" s="62"/>
+      <c r="DR7" s="60"/>
+      <c r="DS7" s="61"/>
+      <c r="DT7" s="61"/>
+      <c r="DU7" s="61"/>
+      <c r="DV7" s="61"/>
+      <c r="DW7" s="61"/>
+      <c r="DX7" s="62"/>
       <c r="DY7" s="2"/>
       <c r="DZ7" s="1"/>
       <c r="EA7" s="1"/>
@@ -2994,15 +2989,15 @@
       <c r="EL7" s="3"/>
     </row>
     <row r="8" spans="1:142" ht="15" thickBot="1">
-      <c r="A8" s="69"/>
-      <c r="B8" s="36" t="s">
+      <c r="A8" s="37"/>
+      <c r="B8" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="64">
+      <c r="D8" s="31">
         <v>2</v>
       </c>
-      <c r="E8" s="64">
+      <c r="E8" s="31">
         <v>2</v>
       </c>
       <c r="F8" s="1"/>
@@ -3010,10 +3005,10 @@
       <c r="H8" s="1"/>
       <c r="I8" s="3"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="64">
+      <c r="K8" s="31">
         <v>2</v>
       </c>
-      <c r="L8" s="64">
+      <c r="L8" s="31">
         <v>2</v>
       </c>
       <c r="M8" s="1"/>
@@ -3036,20 +3031,20 @@
       <c r="AD8" s="3"/>
       <c r="AE8" s="2"/>
       <c r="AF8" s="1"/>
-      <c r="AG8" s="64">
+      <c r="AG8" s="31">
         <v>3</v>
       </c>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="3"/>
-      <c r="AL8" s="57"/>
-      <c r="AM8" s="58"/>
-      <c r="AN8" s="58"/>
-      <c r="AO8" s="58"/>
-      <c r="AP8" s="58"/>
-      <c r="AQ8" s="58"/>
-      <c r="AR8" s="59"/>
+      <c r="AL8" s="52"/>
+      <c r="AM8" s="53"/>
+      <c r="AN8" s="53"/>
+      <c r="AO8" s="53"/>
+      <c r="AP8" s="53"/>
+      <c r="AQ8" s="53"/>
+      <c r="AR8" s="54"/>
       <c r="AS8" s="2"/>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
@@ -3120,20 +3115,20 @@
       <c r="DH8" s="1"/>
       <c r="DI8" s="1"/>
       <c r="DJ8" s="3"/>
-      <c r="DK8" s="48"/>
-      <c r="DL8" s="49"/>
-      <c r="DM8" s="49"/>
-      <c r="DN8" s="49"/>
-      <c r="DO8" s="49"/>
-      <c r="DP8" s="49"/>
-      <c r="DQ8" s="50"/>
-      <c r="DR8" s="48"/>
-      <c r="DS8" s="49"/>
-      <c r="DT8" s="49"/>
-      <c r="DU8" s="49"/>
-      <c r="DV8" s="49"/>
-      <c r="DW8" s="49"/>
-      <c r="DX8" s="50"/>
+      <c r="DK8" s="60"/>
+      <c r="DL8" s="61"/>
+      <c r="DM8" s="61"/>
+      <c r="DN8" s="61"/>
+      <c r="DO8" s="61"/>
+      <c r="DP8" s="61"/>
+      <c r="DQ8" s="62"/>
+      <c r="DR8" s="60"/>
+      <c r="DS8" s="61"/>
+      <c r="DT8" s="61"/>
+      <c r="DU8" s="61"/>
+      <c r="DV8" s="61"/>
+      <c r="DW8" s="61"/>
+      <c r="DX8" s="62"/>
       <c r="DY8" s="2"/>
       <c r="DZ8" s="1"/>
       <c r="EA8" s="1"/>
@@ -3150,10 +3145,10 @@
       <c r="EL8" s="3"/>
     </row>
     <row r="9" spans="1:142" ht="15" thickBot="1">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="2"/>
@@ -3169,13 +3164,13 @@
       <c r="O9" s="1"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="40">
+      <c r="R9" s="26">
         <v>2</v>
       </c>
-      <c r="S9" s="40">
+      <c r="S9" s="26">
         <v>1</v>
       </c>
-      <c r="T9" s="40">
+      <c r="T9" s="26">
         <v>1</v>
       </c>
       <c r="U9" s="1"/>
@@ -3188,20 +3183,20 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="3"/>
-      <c r="AE9" s="41"/>
+      <c r="AE9" s="2"/>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="3"/>
-      <c r="AL9" s="57"/>
-      <c r="AM9" s="58"/>
-      <c r="AN9" s="58"/>
-      <c r="AO9" s="58"/>
-      <c r="AP9" s="58"/>
-      <c r="AQ9" s="58"/>
-      <c r="AR9" s="59"/>
+      <c r="AL9" s="52"/>
+      <c r="AM9" s="53"/>
+      <c r="AN9" s="53"/>
+      <c r="AO9" s="53"/>
+      <c r="AP9" s="53"/>
+      <c r="AQ9" s="53"/>
+      <c r="AR9" s="54"/>
       <c r="AS9" s="2"/>
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
@@ -3272,20 +3267,20 @@
       <c r="DH9" s="1"/>
       <c r="DI9" s="1"/>
       <c r="DJ9" s="3"/>
-      <c r="DK9" s="48"/>
-      <c r="DL9" s="49"/>
-      <c r="DM9" s="49"/>
-      <c r="DN9" s="49"/>
-      <c r="DO9" s="49"/>
-      <c r="DP9" s="49"/>
-      <c r="DQ9" s="50"/>
-      <c r="DR9" s="48"/>
-      <c r="DS9" s="49"/>
-      <c r="DT9" s="49"/>
-      <c r="DU9" s="49"/>
-      <c r="DV9" s="49"/>
-      <c r="DW9" s="49"/>
-      <c r="DX9" s="50"/>
+      <c r="DK9" s="60"/>
+      <c r="DL9" s="61"/>
+      <c r="DM9" s="61"/>
+      <c r="DN9" s="61"/>
+      <c r="DO9" s="61"/>
+      <c r="DP9" s="61"/>
+      <c r="DQ9" s="62"/>
+      <c r="DR9" s="60"/>
+      <c r="DS9" s="61"/>
+      <c r="DT9" s="61"/>
+      <c r="DU9" s="61"/>
+      <c r="DV9" s="61"/>
+      <c r="DW9" s="61"/>
+      <c r="DX9" s="62"/>
       <c r="DY9" s="2"/>
       <c r="DZ9" s="1"/>
       <c r="EA9" s="1"/>
@@ -3302,8 +3297,8 @@
       <c r="EL9" s="3"/>
     </row>
     <row r="10" spans="1:142" ht="15" thickBot="1">
-      <c r="A10" s="67"/>
-      <c r="B10" s="36" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="2"/>
@@ -3321,13 +3316,13 @@
       <c r="O10" s="1"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="64">
+      <c r="R10" s="31">
         <v>2</v>
       </c>
-      <c r="S10" s="64">
+      <c r="S10" s="31">
         <v>2</v>
       </c>
-      <c r="T10" s="64">
+      <c r="T10" s="31">
         <v>2</v>
       </c>
       <c r="U10" s="1"/>
@@ -3347,13 +3342,13 @@
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="3"/>
-      <c r="AL10" s="57"/>
-      <c r="AM10" s="58"/>
-      <c r="AN10" s="58"/>
-      <c r="AO10" s="58"/>
-      <c r="AP10" s="58"/>
-      <c r="AQ10" s="58"/>
-      <c r="AR10" s="59"/>
+      <c r="AL10" s="52"/>
+      <c r="AM10" s="53"/>
+      <c r="AN10" s="53"/>
+      <c r="AO10" s="53"/>
+      <c r="AP10" s="53"/>
+      <c r="AQ10" s="53"/>
+      <c r="AR10" s="54"/>
       <c r="AS10" s="2"/>
       <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
@@ -3424,20 +3419,20 @@
       <c r="DH10" s="1"/>
       <c r="DI10" s="1"/>
       <c r="DJ10" s="3"/>
-      <c r="DK10" s="48"/>
-      <c r="DL10" s="49"/>
-      <c r="DM10" s="49"/>
-      <c r="DN10" s="49"/>
-      <c r="DO10" s="49"/>
-      <c r="DP10" s="49"/>
-      <c r="DQ10" s="50"/>
-      <c r="DR10" s="48"/>
-      <c r="DS10" s="49"/>
-      <c r="DT10" s="49"/>
-      <c r="DU10" s="49"/>
-      <c r="DV10" s="49"/>
-      <c r="DW10" s="49"/>
-      <c r="DX10" s="50"/>
+      <c r="DK10" s="60"/>
+      <c r="DL10" s="61"/>
+      <c r="DM10" s="61"/>
+      <c r="DN10" s="61"/>
+      <c r="DO10" s="61"/>
+      <c r="DP10" s="61"/>
+      <c r="DQ10" s="62"/>
+      <c r="DR10" s="60"/>
+      <c r="DS10" s="61"/>
+      <c r="DT10" s="61"/>
+      <c r="DU10" s="61"/>
+      <c r="DV10" s="61"/>
+      <c r="DW10" s="61"/>
+      <c r="DX10" s="62"/>
       <c r="DY10" s="2"/>
       <c r="DZ10" s="1"/>
       <c r="EA10" s="1"/>
@@ -3454,10 +3449,10 @@
       <c r="EL10" s="3"/>
     </row>
     <row r="11" spans="1:142" ht="15" thickBot="1">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="2"/>
@@ -3483,13 +3478,13 @@
       <c r="W11" s="3"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="40">
+      <c r="Z11" s="26">
         <v>1</v>
       </c>
-      <c r="AA11" s="40">
+      <c r="AA11" s="26">
         <v>1</v>
       </c>
-      <c r="AB11" s="40">
+      <c r="AB11" s="26">
         <v>1</v>
       </c>
       <c r="AC11" s="1"/>
@@ -3501,13 +3496,13 @@
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="3"/>
-      <c r="AL11" s="57"/>
-      <c r="AM11" s="58"/>
-      <c r="AN11" s="58"/>
-      <c r="AO11" s="58"/>
-      <c r="AP11" s="58"/>
-      <c r="AQ11" s="58"/>
-      <c r="AR11" s="59"/>
+      <c r="AL11" s="52"/>
+      <c r="AM11" s="53"/>
+      <c r="AN11" s="53"/>
+      <c r="AO11" s="53"/>
+      <c r="AP11" s="53"/>
+      <c r="AQ11" s="53"/>
+      <c r="AR11" s="54"/>
       <c r="AS11" s="2"/>
       <c r="AT11" s="1"/>
       <c r="AU11" s="1"/>
@@ -3578,20 +3573,20 @@
       <c r="DH11" s="1"/>
       <c r="DI11" s="1"/>
       <c r="DJ11" s="3"/>
-      <c r="DK11" s="48"/>
-      <c r="DL11" s="49"/>
-      <c r="DM11" s="49"/>
-      <c r="DN11" s="49"/>
-      <c r="DO11" s="49"/>
-      <c r="DP11" s="49"/>
-      <c r="DQ11" s="50"/>
-      <c r="DR11" s="48"/>
-      <c r="DS11" s="49"/>
-      <c r="DT11" s="49"/>
-      <c r="DU11" s="49"/>
-      <c r="DV11" s="49"/>
-      <c r="DW11" s="49"/>
-      <c r="DX11" s="50"/>
+      <c r="DK11" s="60"/>
+      <c r="DL11" s="61"/>
+      <c r="DM11" s="61"/>
+      <c r="DN11" s="61"/>
+      <c r="DO11" s="61"/>
+      <c r="DP11" s="61"/>
+      <c r="DQ11" s="62"/>
+      <c r="DR11" s="60"/>
+      <c r="DS11" s="61"/>
+      <c r="DT11" s="61"/>
+      <c r="DU11" s="61"/>
+      <c r="DV11" s="61"/>
+      <c r="DW11" s="61"/>
+      <c r="DX11" s="62"/>
       <c r="DY11" s="2"/>
       <c r="DZ11" s="1"/>
       <c r="EA11" s="1"/>
@@ -3608,8 +3603,8 @@
       <c r="EL11" s="3"/>
     </row>
     <row r="12" spans="1:142" ht="15" thickBot="1">
-      <c r="A12" s="67"/>
-      <c r="B12" s="36" t="s">
+      <c r="A12" s="40"/>
+      <c r="B12" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="2"/>
@@ -3635,13 +3630,13 @@
       <c r="W12" s="3"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="64">
+      <c r="Z12" s="31">
         <v>2</v>
       </c>
-      <c r="AA12" s="64">
+      <c r="AA12" s="31">
         <v>2</v>
       </c>
-      <c r="AB12" s="64">
+      <c r="AB12" s="31">
         <v>1</v>
       </c>
       <c r="AC12" s="1"/>
@@ -3653,13 +3648,13 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="3"/>
-      <c r="AL12" s="57"/>
-      <c r="AM12" s="58"/>
-      <c r="AN12" s="58"/>
-      <c r="AO12" s="58"/>
-      <c r="AP12" s="58"/>
-      <c r="AQ12" s="58"/>
-      <c r="AR12" s="59"/>
+      <c r="AL12" s="52"/>
+      <c r="AM12" s="53"/>
+      <c r="AN12" s="53"/>
+      <c r="AO12" s="53"/>
+      <c r="AP12" s="53"/>
+      <c r="AQ12" s="53"/>
+      <c r="AR12" s="54"/>
       <c r="AS12" s="2"/>
       <c r="AT12" s="1"/>
       <c r="AU12" s="1"/>
@@ -3730,20 +3725,20 @@
       <c r="DH12" s="1"/>
       <c r="DI12" s="1"/>
       <c r="DJ12" s="3"/>
-      <c r="DK12" s="48"/>
-      <c r="DL12" s="49"/>
-      <c r="DM12" s="49"/>
-      <c r="DN12" s="49"/>
-      <c r="DO12" s="49"/>
-      <c r="DP12" s="49"/>
-      <c r="DQ12" s="50"/>
-      <c r="DR12" s="48"/>
-      <c r="DS12" s="49"/>
-      <c r="DT12" s="49"/>
-      <c r="DU12" s="49"/>
-      <c r="DV12" s="49"/>
-      <c r="DW12" s="49"/>
-      <c r="DX12" s="50"/>
+      <c r="DK12" s="60"/>
+      <c r="DL12" s="61"/>
+      <c r="DM12" s="61"/>
+      <c r="DN12" s="61"/>
+      <c r="DO12" s="61"/>
+      <c r="DP12" s="61"/>
+      <c r="DQ12" s="62"/>
+      <c r="DR12" s="60"/>
+      <c r="DS12" s="61"/>
+      <c r="DT12" s="61"/>
+      <c r="DU12" s="61"/>
+      <c r="DV12" s="61"/>
+      <c r="DW12" s="61"/>
+      <c r="DX12" s="62"/>
       <c r="DY12" s="2"/>
       <c r="DZ12" s="1"/>
       <c r="EA12" s="1"/>
@@ -3760,10 +3755,10 @@
       <c r="EL12" s="3"/>
     </row>
     <row r="13" spans="1:142" ht="15" thickBot="1">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="2"/>
@@ -3796,24 +3791,24 @@
       <c r="AD13" s="3"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="1"/>
-      <c r="AG13" s="40">
+      <c r="AG13" s="26">
         <v>1</v>
       </c>
-      <c r="AH13" s="40">
+      <c r="AH13" s="26">
         <v>1</v>
       </c>
-      <c r="AI13" s="40">
+      <c r="AI13" s="26">
         <v>1</v>
       </c>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="3"/>
-      <c r="AL13" s="57"/>
-      <c r="AM13" s="58"/>
-      <c r="AN13" s="58"/>
-      <c r="AO13" s="58"/>
-      <c r="AP13" s="58"/>
-      <c r="AQ13" s="58"/>
-      <c r="AR13" s="59"/>
+      <c r="AL13" s="52"/>
+      <c r="AM13" s="53"/>
+      <c r="AN13" s="53"/>
+      <c r="AO13" s="53"/>
+      <c r="AP13" s="53"/>
+      <c r="AQ13" s="53"/>
+      <c r="AR13" s="54"/>
       <c r="AS13" s="2"/>
       <c r="AT13" s="1"/>
       <c r="AU13" s="1"/>
@@ -3884,20 +3879,20 @@
       <c r="DH13" s="1"/>
       <c r="DI13" s="1"/>
       <c r="DJ13" s="3"/>
-      <c r="DK13" s="48"/>
-      <c r="DL13" s="49"/>
-      <c r="DM13" s="49"/>
-      <c r="DN13" s="49"/>
-      <c r="DO13" s="49"/>
-      <c r="DP13" s="49"/>
-      <c r="DQ13" s="50"/>
-      <c r="DR13" s="48"/>
-      <c r="DS13" s="49"/>
-      <c r="DT13" s="49"/>
-      <c r="DU13" s="49"/>
-      <c r="DV13" s="49"/>
-      <c r="DW13" s="49"/>
-      <c r="DX13" s="50"/>
+      <c r="DK13" s="60"/>
+      <c r="DL13" s="61"/>
+      <c r="DM13" s="61"/>
+      <c r="DN13" s="61"/>
+      <c r="DO13" s="61"/>
+      <c r="DP13" s="61"/>
+      <c r="DQ13" s="62"/>
+      <c r="DR13" s="60"/>
+      <c r="DS13" s="61"/>
+      <c r="DT13" s="61"/>
+      <c r="DU13" s="61"/>
+      <c r="DV13" s="61"/>
+      <c r="DW13" s="61"/>
+      <c r="DX13" s="62"/>
       <c r="DY13" s="2"/>
       <c r="DZ13" s="1"/>
       <c r="EA13" s="1"/>
@@ -3914,8 +3909,8 @@
       <c r="EL13" s="3"/>
     </row>
     <row r="14" spans="1:142" ht="15" thickBot="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="36" t="s">
+      <c r="A14" s="37"/>
+      <c r="B14" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="2"/>
@@ -3953,13 +3948,13 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="3"/>
-      <c r="AL14" s="57"/>
-      <c r="AM14" s="58"/>
-      <c r="AN14" s="58"/>
-      <c r="AO14" s="58"/>
-      <c r="AP14" s="58"/>
-      <c r="AQ14" s="58"/>
-      <c r="AR14" s="59"/>
+      <c r="AL14" s="52"/>
+      <c r="AM14" s="53"/>
+      <c r="AN14" s="53"/>
+      <c r="AO14" s="53"/>
+      <c r="AP14" s="53"/>
+      <c r="AQ14" s="53"/>
+      <c r="AR14" s="54"/>
       <c r="AS14" s="2"/>
       <c r="AT14" s="1"/>
       <c r="AU14" s="1"/>
@@ -4030,20 +4025,20 @@
       <c r="DH14" s="1"/>
       <c r="DI14" s="1"/>
       <c r="DJ14" s="3"/>
-      <c r="DK14" s="48"/>
-      <c r="DL14" s="49"/>
-      <c r="DM14" s="49"/>
-      <c r="DN14" s="49"/>
-      <c r="DO14" s="49"/>
-      <c r="DP14" s="49"/>
-      <c r="DQ14" s="50"/>
-      <c r="DR14" s="48"/>
-      <c r="DS14" s="49"/>
-      <c r="DT14" s="49"/>
-      <c r="DU14" s="49"/>
-      <c r="DV14" s="49"/>
-      <c r="DW14" s="49"/>
-      <c r="DX14" s="50"/>
+      <c r="DK14" s="60"/>
+      <c r="DL14" s="61"/>
+      <c r="DM14" s="61"/>
+      <c r="DN14" s="61"/>
+      <c r="DO14" s="61"/>
+      <c r="DP14" s="61"/>
+      <c r="DQ14" s="62"/>
+      <c r="DR14" s="60"/>
+      <c r="DS14" s="61"/>
+      <c r="DT14" s="61"/>
+      <c r="DU14" s="61"/>
+      <c r="DV14" s="61"/>
+      <c r="DW14" s="61"/>
+      <c r="DX14" s="62"/>
       <c r="DY14" s="2"/>
       <c r="DZ14" s="1"/>
       <c r="EA14" s="1"/>
@@ -4060,10 +4055,10 @@
       <c r="EL14" s="3"/>
     </row>
     <row r="15" spans="1:142" ht="15" thickBot="1">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="2"/>
@@ -4101,22 +4096,22 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="3"/>
-      <c r="AL15" s="57"/>
-      <c r="AM15" s="58"/>
-      <c r="AN15" s="58"/>
-      <c r="AO15" s="58"/>
-      <c r="AP15" s="58"/>
-      <c r="AQ15" s="58"/>
-      <c r="AR15" s="59"/>
+      <c r="AL15" s="52"/>
+      <c r="AM15" s="53"/>
+      <c r="AN15" s="53"/>
+      <c r="AO15" s="53"/>
+      <c r="AP15" s="53"/>
+      <c r="AQ15" s="53"/>
+      <c r="AR15" s="54"/>
       <c r="AS15" s="2"/>
       <c r="AT15" s="1"/>
-      <c r="AU15" s="40">
+      <c r="AU15" s="26">
         <v>2</v>
       </c>
-      <c r="AV15" s="40">
+      <c r="AV15" s="26">
         <v>2</v>
       </c>
-      <c r="AW15" s="40">
+      <c r="AW15" s="26">
         <v>2</v>
       </c>
       <c r="AX15" s="1"/>
@@ -4184,20 +4179,20 @@
       <c r="DH15" s="1"/>
       <c r="DI15" s="1"/>
       <c r="DJ15" s="3"/>
-      <c r="DK15" s="48"/>
-      <c r="DL15" s="49"/>
-      <c r="DM15" s="49"/>
-      <c r="DN15" s="49"/>
-      <c r="DO15" s="49"/>
-      <c r="DP15" s="49"/>
-      <c r="DQ15" s="50"/>
-      <c r="DR15" s="48"/>
-      <c r="DS15" s="49"/>
-      <c r="DT15" s="49"/>
-      <c r="DU15" s="49"/>
-      <c r="DV15" s="49"/>
-      <c r="DW15" s="49"/>
-      <c r="DX15" s="50"/>
+      <c r="DK15" s="60"/>
+      <c r="DL15" s="61"/>
+      <c r="DM15" s="61"/>
+      <c r="DN15" s="61"/>
+      <c r="DO15" s="61"/>
+      <c r="DP15" s="61"/>
+      <c r="DQ15" s="62"/>
+      <c r="DR15" s="60"/>
+      <c r="DS15" s="61"/>
+      <c r="DT15" s="61"/>
+      <c r="DU15" s="61"/>
+      <c r="DV15" s="61"/>
+      <c r="DW15" s="61"/>
+      <c r="DX15" s="62"/>
       <c r="DY15" s="2"/>
       <c r="DZ15" s="1"/>
       <c r="EA15" s="1"/>
@@ -4214,8 +4209,8 @@
       <c r="EL15" s="3"/>
     </row>
     <row r="16" spans="1:142" ht="15" thickBot="1">
-      <c r="A16" s="71"/>
-      <c r="B16" s="36" t="s">
+      <c r="A16" s="41"/>
+      <c r="B16" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="2"/>
@@ -4253,13 +4248,13 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="3"/>
-      <c r="AL16" s="57"/>
-      <c r="AM16" s="58"/>
-      <c r="AN16" s="58"/>
-      <c r="AO16" s="58"/>
-      <c r="AP16" s="58"/>
-      <c r="AQ16" s="58"/>
-      <c r="AR16" s="59"/>
+      <c r="AL16" s="52"/>
+      <c r="AM16" s="53"/>
+      <c r="AN16" s="53"/>
+      <c r="AO16" s="53"/>
+      <c r="AP16" s="53"/>
+      <c r="AQ16" s="53"/>
+      <c r="AR16" s="54"/>
       <c r="AS16" s="2"/>
       <c r="AT16" s="1"/>
       <c r="AU16" s="1"/>
@@ -4330,20 +4325,20 @@
       <c r="DH16" s="1"/>
       <c r="DI16" s="1"/>
       <c r="DJ16" s="3"/>
-      <c r="DK16" s="48"/>
-      <c r="DL16" s="49"/>
-      <c r="DM16" s="49"/>
-      <c r="DN16" s="49"/>
-      <c r="DO16" s="49"/>
-      <c r="DP16" s="49"/>
-      <c r="DQ16" s="50"/>
-      <c r="DR16" s="48"/>
-      <c r="DS16" s="49"/>
-      <c r="DT16" s="49"/>
-      <c r="DU16" s="49"/>
-      <c r="DV16" s="49"/>
-      <c r="DW16" s="49"/>
-      <c r="DX16" s="50"/>
+      <c r="DK16" s="60"/>
+      <c r="DL16" s="61"/>
+      <c r="DM16" s="61"/>
+      <c r="DN16" s="61"/>
+      <c r="DO16" s="61"/>
+      <c r="DP16" s="61"/>
+      <c r="DQ16" s="62"/>
+      <c r="DR16" s="60"/>
+      <c r="DS16" s="61"/>
+      <c r="DT16" s="61"/>
+      <c r="DU16" s="61"/>
+      <c r="DV16" s="61"/>
+      <c r="DW16" s="61"/>
+      <c r="DX16" s="62"/>
       <c r="DY16" s="2"/>
       <c r="DZ16" s="1"/>
       <c r="EA16" s="1"/>
@@ -4360,10 +4355,10 @@
       <c r="EL16" s="3"/>
     </row>
     <row r="17" spans="1:142" ht="15" thickBot="1">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="2"/>
@@ -4401,25 +4396,25 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="3"/>
-      <c r="AL17" s="57"/>
-      <c r="AM17" s="58"/>
-      <c r="AN17" s="58"/>
-      <c r="AO17" s="58"/>
-      <c r="AP17" s="58"/>
-      <c r="AQ17" s="58"/>
-      <c r="AR17" s="59"/>
+      <c r="AL17" s="52"/>
+      <c r="AM17" s="53"/>
+      <c r="AN17" s="53"/>
+      <c r="AO17" s="53"/>
+      <c r="AP17" s="53"/>
+      <c r="AQ17" s="53"/>
+      <c r="AR17" s="54"/>
       <c r="AS17" s="2"/>
       <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
-      <c r="AW17" s="40">
+      <c r="AW17" s="26">
         <v>1</v>
       </c>
       <c r="AX17" s="1"/>
       <c r="AY17" s="3"/>
       <c r="AZ17" s="2"/>
       <c r="BA17" s="1"/>
-      <c r="BB17" s="40">
+      <c r="BB17" s="26">
         <v>2</v>
       </c>
       <c r="BD17" s="1"/>
@@ -4481,20 +4476,20 @@
       <c r="DH17" s="1"/>
       <c r="DI17" s="1"/>
       <c r="DJ17" s="3"/>
-      <c r="DK17" s="48"/>
-      <c r="DL17" s="49"/>
-      <c r="DM17" s="49"/>
-      <c r="DN17" s="49"/>
-      <c r="DO17" s="49"/>
-      <c r="DP17" s="49"/>
-      <c r="DQ17" s="50"/>
-      <c r="DR17" s="48"/>
-      <c r="DS17" s="49"/>
-      <c r="DT17" s="49"/>
-      <c r="DU17" s="49"/>
-      <c r="DV17" s="49"/>
-      <c r="DW17" s="49"/>
-      <c r="DX17" s="50"/>
+      <c r="DK17" s="60"/>
+      <c r="DL17" s="61"/>
+      <c r="DM17" s="61"/>
+      <c r="DN17" s="61"/>
+      <c r="DO17" s="61"/>
+      <c r="DP17" s="61"/>
+      <c r="DQ17" s="62"/>
+      <c r="DR17" s="60"/>
+      <c r="DS17" s="61"/>
+      <c r="DT17" s="61"/>
+      <c r="DU17" s="61"/>
+      <c r="DV17" s="61"/>
+      <c r="DW17" s="61"/>
+      <c r="DX17" s="62"/>
       <c r="DY17" s="2"/>
       <c r="DZ17" s="1"/>
       <c r="EA17" s="1"/>
@@ -4511,8 +4506,8 @@
       <c r="EL17" s="3"/>
     </row>
     <row r="18" spans="1:142" ht="15" thickBot="1">
-      <c r="A18" s="71"/>
-      <c r="B18" s="36" t="s">
+      <c r="A18" s="41"/>
+      <c r="B18" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="2"/>
@@ -4550,13 +4545,13 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="3"/>
-      <c r="AL18" s="57"/>
-      <c r="AM18" s="58"/>
-      <c r="AN18" s="58"/>
-      <c r="AO18" s="58"/>
-      <c r="AP18" s="58"/>
-      <c r="AQ18" s="58"/>
-      <c r="AR18" s="59"/>
+      <c r="AL18" s="52"/>
+      <c r="AM18" s="53"/>
+      <c r="AN18" s="53"/>
+      <c r="AO18" s="53"/>
+      <c r="AP18" s="53"/>
+      <c r="AQ18" s="53"/>
+      <c r="AR18" s="54"/>
       <c r="AS18" s="2"/>
       <c r="AT18" s="1"/>
       <c r="AU18" s="1"/>
@@ -4627,20 +4622,20 @@
       <c r="DH18" s="1"/>
       <c r="DI18" s="1"/>
       <c r="DJ18" s="3"/>
-      <c r="DK18" s="48"/>
-      <c r="DL18" s="49"/>
-      <c r="DM18" s="49"/>
-      <c r="DN18" s="49"/>
-      <c r="DO18" s="49"/>
-      <c r="DP18" s="49"/>
-      <c r="DQ18" s="50"/>
-      <c r="DR18" s="48"/>
-      <c r="DS18" s="49"/>
-      <c r="DT18" s="49"/>
-      <c r="DU18" s="49"/>
-      <c r="DV18" s="49"/>
-      <c r="DW18" s="49"/>
-      <c r="DX18" s="50"/>
+      <c r="DK18" s="60"/>
+      <c r="DL18" s="61"/>
+      <c r="DM18" s="61"/>
+      <c r="DN18" s="61"/>
+      <c r="DO18" s="61"/>
+      <c r="DP18" s="61"/>
+      <c r="DQ18" s="62"/>
+      <c r="DR18" s="60"/>
+      <c r="DS18" s="61"/>
+      <c r="DT18" s="61"/>
+      <c r="DU18" s="61"/>
+      <c r="DV18" s="61"/>
+      <c r="DW18" s="61"/>
+      <c r="DX18" s="62"/>
       <c r="DY18" s="2"/>
       <c r="DZ18" s="1"/>
       <c r="EA18" s="1"/>
@@ -4657,10 +4652,10 @@
       <c r="EL18" s="3"/>
     </row>
     <row r="19" spans="1:142" ht="15" thickBot="1">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="2"/>
@@ -4698,29 +4693,29 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="3"/>
-      <c r="AL19" s="57"/>
-      <c r="AM19" s="58"/>
-      <c r="AN19" s="58"/>
-      <c r="AO19" s="58"/>
-      <c r="AP19" s="58"/>
-      <c r="AQ19" s="58"/>
-      <c r="AR19" s="59"/>
+      <c r="AL19" s="52"/>
+      <c r="AM19" s="53"/>
+      <c r="AN19" s="53"/>
+      <c r="AO19" s="53"/>
+      <c r="AP19" s="53"/>
+      <c r="AQ19" s="53"/>
+      <c r="AR19" s="54"/>
       <c r="AS19" s="2"/>
       <c r="AT19" s="1"/>
       <c r="AU19" s="1"/>
-      <c r="AV19" s="34"/>
-      <c r="AW19" s="34"/>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="1"/>
       <c r="AX19" s="1"/>
       <c r="AY19" s="3"/>
       <c r="AZ19" s="2"/>
       <c r="BA19" s="1"/>
-      <c r="BB19" s="40">
+      <c r="BB19" s="26">
         <v>2</v>
       </c>
-      <c r="BC19" s="40">
+      <c r="BC19" s="26">
         <v>2</v>
       </c>
-      <c r="BD19" s="40">
+      <c r="BD19" s="26">
         <v>2</v>
       </c>
       <c r="BE19" s="1"/>
@@ -4781,20 +4776,20 @@
       <c r="DH19" s="1"/>
       <c r="DI19" s="1"/>
       <c r="DJ19" s="3"/>
-      <c r="DK19" s="48"/>
-      <c r="DL19" s="49"/>
-      <c r="DM19" s="49"/>
-      <c r="DN19" s="49"/>
-      <c r="DO19" s="49"/>
-      <c r="DP19" s="49"/>
-      <c r="DQ19" s="50"/>
-      <c r="DR19" s="48"/>
-      <c r="DS19" s="49"/>
-      <c r="DT19" s="49"/>
-      <c r="DU19" s="49"/>
-      <c r="DV19" s="49"/>
-      <c r="DW19" s="49"/>
-      <c r="DX19" s="50"/>
+      <c r="DK19" s="60"/>
+      <c r="DL19" s="61"/>
+      <c r="DM19" s="61"/>
+      <c r="DN19" s="61"/>
+      <c r="DO19" s="61"/>
+      <c r="DP19" s="61"/>
+      <c r="DQ19" s="62"/>
+      <c r="DR19" s="60"/>
+      <c r="DS19" s="61"/>
+      <c r="DT19" s="61"/>
+      <c r="DU19" s="61"/>
+      <c r="DV19" s="61"/>
+      <c r="DW19" s="61"/>
+      <c r="DX19" s="62"/>
       <c r="DY19" s="2"/>
       <c r="DZ19" s="1"/>
       <c r="EA19" s="1"/>
@@ -4811,8 +4806,8 @@
       <c r="EL19" s="3"/>
     </row>
     <row r="20" spans="1:142" ht="15" thickBot="1">
-      <c r="A20" s="71"/>
-      <c r="B20" s="36" t="s">
+      <c r="A20" s="41"/>
+      <c r="B20" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="2"/>
@@ -4850,13 +4845,13 @@
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="3"/>
-      <c r="AL20" s="57"/>
-      <c r="AM20" s="58"/>
-      <c r="AN20" s="58"/>
-      <c r="AO20" s="58"/>
-      <c r="AP20" s="58"/>
-      <c r="AQ20" s="58"/>
-      <c r="AR20" s="59"/>
+      <c r="AL20" s="52"/>
+      <c r="AM20" s="53"/>
+      <c r="AN20" s="53"/>
+      <c r="AO20" s="53"/>
+      <c r="AP20" s="53"/>
+      <c r="AQ20" s="53"/>
+      <c r="AR20" s="54"/>
       <c r="AS20" s="2"/>
       <c r="AT20" s="1"/>
       <c r="AU20" s="1"/>
@@ -4927,20 +4922,20 @@
       <c r="DH20" s="1"/>
       <c r="DI20" s="1"/>
       <c r="DJ20" s="3"/>
-      <c r="DK20" s="48"/>
-      <c r="DL20" s="49"/>
-      <c r="DM20" s="49"/>
-      <c r="DN20" s="49"/>
-      <c r="DO20" s="49"/>
-      <c r="DP20" s="49"/>
-      <c r="DQ20" s="50"/>
-      <c r="DR20" s="48"/>
-      <c r="DS20" s="49"/>
-      <c r="DT20" s="49"/>
-      <c r="DU20" s="49"/>
-      <c r="DV20" s="49"/>
-      <c r="DW20" s="49"/>
-      <c r="DX20" s="50"/>
+      <c r="DK20" s="60"/>
+      <c r="DL20" s="61"/>
+      <c r="DM20" s="61"/>
+      <c r="DN20" s="61"/>
+      <c r="DO20" s="61"/>
+      <c r="DP20" s="61"/>
+      <c r="DQ20" s="62"/>
+      <c r="DR20" s="60"/>
+      <c r="DS20" s="61"/>
+      <c r="DT20" s="61"/>
+      <c r="DU20" s="61"/>
+      <c r="DV20" s="61"/>
+      <c r="DW20" s="61"/>
+      <c r="DX20" s="62"/>
       <c r="DY20" s="2"/>
       <c r="DZ20" s="1"/>
       <c r="EA20" s="1"/>
@@ -4957,10 +4952,10 @@
       <c r="EL20" s="3"/>
     </row>
     <row r="21" spans="1:142" ht="15" thickBot="1">
-      <c r="A21" s="68" t="s">
+      <c r="A21" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="2"/>
@@ -4998,13 +4993,13 @@
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="3"/>
-      <c r="AL21" s="57"/>
-      <c r="AM21" s="58"/>
-      <c r="AN21" s="58"/>
-      <c r="AO21" s="58"/>
-      <c r="AP21" s="58"/>
-      <c r="AQ21" s="58"/>
-      <c r="AR21" s="59"/>
+      <c r="AL21" s="52"/>
+      <c r="AM21" s="53"/>
+      <c r="AN21" s="53"/>
+      <c r="AO21" s="53"/>
+      <c r="AP21" s="53"/>
+      <c r="AQ21" s="53"/>
+      <c r="AR21" s="54"/>
       <c r="AS21" s="2"/>
       <c r="AT21" s="1"/>
       <c r="AU21" s="1"/>
@@ -5021,14 +5016,14 @@
       <c r="BF21" s="3"/>
       <c r="BG21" s="2"/>
       <c r="BH21" s="1"/>
-      <c r="BI21" s="40">
-        <v>1</v>
-      </c>
-      <c r="BJ21" s="40">
-        <v>1</v>
-      </c>
-      <c r="BK21" s="40">
-        <v>1</v>
+      <c r="BI21" s="26">
+        <v>4</v>
+      </c>
+      <c r="BJ21" s="26">
+        <v>2</v>
+      </c>
+      <c r="BK21" s="26">
+        <v>2</v>
       </c>
       <c r="BL21" s="1"/>
       <c r="BM21" s="3"/>
@@ -5081,20 +5076,20 @@
       <c r="DH21" s="1"/>
       <c r="DI21" s="1"/>
       <c r="DJ21" s="3"/>
-      <c r="DK21" s="48"/>
-      <c r="DL21" s="49"/>
-      <c r="DM21" s="49"/>
-      <c r="DN21" s="49"/>
-      <c r="DO21" s="49"/>
-      <c r="DP21" s="49"/>
-      <c r="DQ21" s="50"/>
-      <c r="DR21" s="48"/>
-      <c r="DS21" s="49"/>
-      <c r="DT21" s="49"/>
-      <c r="DU21" s="49"/>
-      <c r="DV21" s="49"/>
-      <c r="DW21" s="49"/>
-      <c r="DX21" s="50"/>
+      <c r="DK21" s="60"/>
+      <c r="DL21" s="61"/>
+      <c r="DM21" s="61"/>
+      <c r="DN21" s="61"/>
+      <c r="DO21" s="61"/>
+      <c r="DP21" s="61"/>
+      <c r="DQ21" s="62"/>
+      <c r="DR21" s="60"/>
+      <c r="DS21" s="61"/>
+      <c r="DT21" s="61"/>
+      <c r="DU21" s="61"/>
+      <c r="DV21" s="61"/>
+      <c r="DW21" s="61"/>
+      <c r="DX21" s="62"/>
       <c r="DY21" s="2"/>
       <c r="DZ21" s="1"/>
       <c r="EA21" s="1"/>
@@ -5111,8 +5106,8 @@
       <c r="EL21" s="3"/>
     </row>
     <row r="22" spans="1:142" ht="15" thickBot="1">
-      <c r="A22" s="69"/>
-      <c r="B22" s="36" t="s">
+      <c r="A22" s="37"/>
+      <c r="B22" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="2"/>
@@ -5150,13 +5145,13 @@
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="3"/>
-      <c r="AL22" s="57"/>
-      <c r="AM22" s="58"/>
-      <c r="AN22" s="58"/>
-      <c r="AO22" s="58"/>
-      <c r="AP22" s="58"/>
-      <c r="AQ22" s="58"/>
-      <c r="AR22" s="59"/>
+      <c r="AL22" s="52"/>
+      <c r="AM22" s="53"/>
+      <c r="AN22" s="53"/>
+      <c r="AO22" s="53"/>
+      <c r="AP22" s="53"/>
+      <c r="AQ22" s="53"/>
+      <c r="AR22" s="54"/>
       <c r="AS22" s="2"/>
       <c r="AT22" s="1"/>
       <c r="AU22" s="1"/>
@@ -5227,20 +5222,20 @@
       <c r="DH22" s="1"/>
       <c r="DI22" s="1"/>
       <c r="DJ22" s="3"/>
-      <c r="DK22" s="48"/>
-      <c r="DL22" s="49"/>
-      <c r="DM22" s="49"/>
-      <c r="DN22" s="49"/>
-      <c r="DO22" s="49"/>
-      <c r="DP22" s="49"/>
-      <c r="DQ22" s="50"/>
-      <c r="DR22" s="48"/>
-      <c r="DS22" s="49"/>
-      <c r="DT22" s="49"/>
-      <c r="DU22" s="49"/>
-      <c r="DV22" s="49"/>
-      <c r="DW22" s="49"/>
-      <c r="DX22" s="50"/>
+      <c r="DK22" s="60"/>
+      <c r="DL22" s="61"/>
+      <c r="DM22" s="61"/>
+      <c r="DN22" s="61"/>
+      <c r="DO22" s="61"/>
+      <c r="DP22" s="61"/>
+      <c r="DQ22" s="62"/>
+      <c r="DR22" s="60"/>
+      <c r="DS22" s="61"/>
+      <c r="DT22" s="61"/>
+      <c r="DU22" s="61"/>
+      <c r="DV22" s="61"/>
+      <c r="DW22" s="61"/>
+      <c r="DX22" s="62"/>
       <c r="DY22" s="2"/>
       <c r="DZ22" s="1"/>
       <c r="EA22" s="1"/>
@@ -5257,10 +5252,10 @@
       <c r="EL22" s="3"/>
     </row>
     <row r="23" spans="1:142" ht="15" thickBot="1">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="2"/>
@@ -5298,13 +5293,13 @@
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="3"/>
-      <c r="AL23" s="57"/>
-      <c r="AM23" s="58"/>
-      <c r="AN23" s="58"/>
-      <c r="AO23" s="58"/>
-      <c r="AP23" s="58"/>
-      <c r="AQ23" s="58"/>
-      <c r="AR23" s="59"/>
+      <c r="AL23" s="52"/>
+      <c r="AM23" s="53"/>
+      <c r="AN23" s="53"/>
+      <c r="AO23" s="53"/>
+      <c r="AP23" s="53"/>
+      <c r="AQ23" s="53"/>
+      <c r="AR23" s="54"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="1"/>
       <c r="AU23" s="1"/>
@@ -5323,7 +5318,7 @@
       <c r="BH23" s="1"/>
       <c r="BI23" s="1"/>
       <c r="BJ23" s="1"/>
-      <c r="BK23" s="40">
+      <c r="BK23" s="26">
         <v>4</v>
       </c>
       <c r="BL23" s="1"/>
@@ -5377,20 +5372,20 @@
       <c r="DH23" s="1"/>
       <c r="DI23" s="1"/>
       <c r="DJ23" s="3"/>
-      <c r="DK23" s="48"/>
-      <c r="DL23" s="49"/>
-      <c r="DM23" s="49"/>
-      <c r="DN23" s="49"/>
-      <c r="DO23" s="49"/>
-      <c r="DP23" s="49"/>
-      <c r="DQ23" s="50"/>
-      <c r="DR23" s="48"/>
-      <c r="DS23" s="49"/>
-      <c r="DT23" s="49"/>
-      <c r="DU23" s="49"/>
-      <c r="DV23" s="49"/>
-      <c r="DW23" s="49"/>
-      <c r="DX23" s="50"/>
+      <c r="DK23" s="60"/>
+      <c r="DL23" s="61"/>
+      <c r="DM23" s="61"/>
+      <c r="DN23" s="61"/>
+      <c r="DO23" s="61"/>
+      <c r="DP23" s="61"/>
+      <c r="DQ23" s="62"/>
+      <c r="DR23" s="60"/>
+      <c r="DS23" s="61"/>
+      <c r="DT23" s="61"/>
+      <c r="DU23" s="61"/>
+      <c r="DV23" s="61"/>
+      <c r="DW23" s="61"/>
+      <c r="DX23" s="62"/>
       <c r="DY23" s="2"/>
       <c r="DZ23" s="1"/>
       <c r="EA23" s="1"/>
@@ -5407,8 +5402,8 @@
       <c r="EL23" s="3"/>
     </row>
     <row r="24" spans="1:142" ht="15" thickBot="1">
-      <c r="A24" s="69"/>
-      <c r="B24" s="36" t="s">
+      <c r="A24" s="37"/>
+      <c r="B24" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="2"/>
@@ -5446,13 +5441,13 @@
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="3"/>
-      <c r="AL24" s="57"/>
-      <c r="AM24" s="58"/>
-      <c r="AN24" s="58"/>
-      <c r="AO24" s="58"/>
-      <c r="AP24" s="58"/>
-      <c r="AQ24" s="58"/>
-      <c r="AR24" s="59"/>
+      <c r="AL24" s="52"/>
+      <c r="AM24" s="53"/>
+      <c r="AN24" s="53"/>
+      <c r="AO24" s="53"/>
+      <c r="AP24" s="53"/>
+      <c r="AQ24" s="53"/>
+      <c r="AR24" s="54"/>
       <c r="AS24" s="2"/>
       <c r="AT24" s="1"/>
       <c r="AU24" s="1"/>
@@ -5523,20 +5518,20 @@
       <c r="DH24" s="1"/>
       <c r="DI24" s="1"/>
       <c r="DJ24" s="3"/>
-      <c r="DK24" s="48"/>
-      <c r="DL24" s="49"/>
-      <c r="DM24" s="49"/>
-      <c r="DN24" s="49"/>
-      <c r="DO24" s="49"/>
-      <c r="DP24" s="49"/>
-      <c r="DQ24" s="50"/>
-      <c r="DR24" s="48"/>
-      <c r="DS24" s="49"/>
-      <c r="DT24" s="49"/>
-      <c r="DU24" s="49"/>
-      <c r="DV24" s="49"/>
-      <c r="DW24" s="49"/>
-      <c r="DX24" s="50"/>
+      <c r="DK24" s="60"/>
+      <c r="DL24" s="61"/>
+      <c r="DM24" s="61"/>
+      <c r="DN24" s="61"/>
+      <c r="DO24" s="61"/>
+      <c r="DP24" s="61"/>
+      <c r="DQ24" s="62"/>
+      <c r="DR24" s="60"/>
+      <c r="DS24" s="61"/>
+      <c r="DT24" s="61"/>
+      <c r="DU24" s="61"/>
+      <c r="DV24" s="61"/>
+      <c r="DW24" s="61"/>
+      <c r="DX24" s="62"/>
       <c r="DY24" s="2"/>
       <c r="DZ24" s="1"/>
       <c r="EA24" s="1"/>
@@ -5553,10 +5548,10 @@
       <c r="EL24" s="3"/>
     </row>
     <row r="25" spans="1:142" ht="15" thickBot="1">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="2"/>
@@ -5594,13 +5589,13 @@
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="3"/>
-      <c r="AL25" s="57"/>
-      <c r="AM25" s="58"/>
-      <c r="AN25" s="58"/>
-      <c r="AO25" s="58"/>
-      <c r="AP25" s="58"/>
-      <c r="AQ25" s="58"/>
-      <c r="AR25" s="59"/>
+      <c r="AL25" s="52"/>
+      <c r="AM25" s="53"/>
+      <c r="AN25" s="53"/>
+      <c r="AO25" s="53"/>
+      <c r="AP25" s="53"/>
+      <c r="AQ25" s="53"/>
+      <c r="AR25" s="54"/>
       <c r="AS25" s="2"/>
       <c r="AT25" s="1"/>
       <c r="AU25" s="1"/>
@@ -5623,10 +5618,10 @@
       <c r="BL25" s="1"/>
       <c r="BM25" s="3"/>
       <c r="BN25" s="2"/>
-      <c r="BO25" s="40">
+      <c r="BO25" s="26">
         <v>1</v>
       </c>
-      <c r="BP25" s="40">
+      <c r="BP25" s="26">
         <v>1</v>
       </c>
       <c r="BQ25" s="1"/>
@@ -5675,20 +5670,20 @@
       <c r="DH25" s="1"/>
       <c r="DI25" s="1"/>
       <c r="DJ25" s="3"/>
-      <c r="DK25" s="48"/>
-      <c r="DL25" s="49"/>
-      <c r="DM25" s="49"/>
-      <c r="DN25" s="49"/>
-      <c r="DO25" s="49"/>
-      <c r="DP25" s="49"/>
-      <c r="DQ25" s="50"/>
-      <c r="DR25" s="48"/>
-      <c r="DS25" s="49"/>
-      <c r="DT25" s="49"/>
-      <c r="DU25" s="49"/>
-      <c r="DV25" s="49"/>
-      <c r="DW25" s="49"/>
-      <c r="DX25" s="50"/>
+      <c r="DK25" s="60"/>
+      <c r="DL25" s="61"/>
+      <c r="DM25" s="61"/>
+      <c r="DN25" s="61"/>
+      <c r="DO25" s="61"/>
+      <c r="DP25" s="61"/>
+      <c r="DQ25" s="62"/>
+      <c r="DR25" s="60"/>
+      <c r="DS25" s="61"/>
+      <c r="DT25" s="61"/>
+      <c r="DU25" s="61"/>
+      <c r="DV25" s="61"/>
+      <c r="DW25" s="61"/>
+      <c r="DX25" s="62"/>
       <c r="DY25" s="2"/>
       <c r="DZ25" s="1"/>
       <c r="EA25" s="1"/>
@@ -5705,8 +5700,8 @@
       <c r="EL25" s="3"/>
     </row>
     <row r="26" spans="1:142" ht="15" thickBot="1">
-      <c r="A26" s="69"/>
-      <c r="B26" s="36" t="s">
+      <c r="A26" s="37"/>
+      <c r="B26" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="2"/>
@@ -5744,13 +5739,13 @@
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="3"/>
-      <c r="AL26" s="57"/>
-      <c r="AM26" s="58"/>
-      <c r="AN26" s="58"/>
-      <c r="AO26" s="58"/>
-      <c r="AP26" s="58"/>
-      <c r="AQ26" s="58"/>
-      <c r="AR26" s="59"/>
+      <c r="AL26" s="52"/>
+      <c r="AM26" s="53"/>
+      <c r="AN26" s="53"/>
+      <c r="AO26" s="53"/>
+      <c r="AP26" s="53"/>
+      <c r="AQ26" s="53"/>
+      <c r="AR26" s="54"/>
       <c r="AS26" s="2"/>
       <c r="AT26" s="1"/>
       <c r="AU26" s="1"/>
@@ -5789,8 +5784,8 @@
       <c r="CB26" s="2"/>
       <c r="CC26" s="1"/>
       <c r="CD26" s="1"/>
-      <c r="CE26" s="34"/>
-      <c r="CF26" s="34"/>
+      <c r="CE26" s="1"/>
+      <c r="CF26" s="1"/>
       <c r="CG26" s="1"/>
       <c r="CH26" s="3"/>
       <c r="CI26" s="2"/>
@@ -5821,20 +5816,20 @@
       <c r="DH26" s="1"/>
       <c r="DI26" s="1"/>
       <c r="DJ26" s="3"/>
-      <c r="DK26" s="48"/>
-      <c r="DL26" s="49"/>
-      <c r="DM26" s="49"/>
-      <c r="DN26" s="49"/>
-      <c r="DO26" s="49"/>
-      <c r="DP26" s="49"/>
-      <c r="DQ26" s="50"/>
-      <c r="DR26" s="48"/>
-      <c r="DS26" s="49"/>
-      <c r="DT26" s="49"/>
-      <c r="DU26" s="49"/>
-      <c r="DV26" s="49"/>
-      <c r="DW26" s="49"/>
-      <c r="DX26" s="50"/>
+      <c r="DK26" s="60"/>
+      <c r="DL26" s="61"/>
+      <c r="DM26" s="61"/>
+      <c r="DN26" s="61"/>
+      <c r="DO26" s="61"/>
+      <c r="DP26" s="61"/>
+      <c r="DQ26" s="62"/>
+      <c r="DR26" s="60"/>
+      <c r="DS26" s="61"/>
+      <c r="DT26" s="61"/>
+      <c r="DU26" s="61"/>
+      <c r="DV26" s="61"/>
+      <c r="DW26" s="61"/>
+      <c r="DX26" s="62"/>
       <c r="DY26" s="2"/>
       <c r="DZ26" s="1"/>
       <c r="EA26" s="1"/>
@@ -5851,10 +5846,10 @@
       <c r="EL26" s="3"/>
     </row>
     <row r="27" spans="1:142" ht="15" thickBot="1">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="2"/>
@@ -5892,13 +5887,13 @@
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="3"/>
-      <c r="AL27" s="57"/>
-      <c r="AM27" s="58"/>
-      <c r="AN27" s="58"/>
-      <c r="AO27" s="58"/>
-      <c r="AP27" s="58"/>
-      <c r="AQ27" s="58"/>
-      <c r="AR27" s="59"/>
+      <c r="AL27" s="52"/>
+      <c r="AM27" s="53"/>
+      <c r="AN27" s="53"/>
+      <c r="AO27" s="53"/>
+      <c r="AP27" s="53"/>
+      <c r="AQ27" s="53"/>
+      <c r="AR27" s="54"/>
       <c r="AS27" s="2"/>
       <c r="AT27" s="1"/>
       <c r="AU27" s="1"/>
@@ -5922,22 +5917,22 @@
       <c r="BM27" s="3"/>
       <c r="BN27" s="2"/>
       <c r="BO27" s="1"/>
-      <c r="BP27" s="40">
+      <c r="BP27" s="26">
         <v>2</v>
       </c>
-      <c r="BQ27" s="40">
+      <c r="BQ27" s="26">
         <v>2</v>
       </c>
-      <c r="BR27" s="40">
+      <c r="BR27" s="26">
         <v>2</v>
       </c>
       <c r="BS27" s="1"/>
       <c r="BT27" s="3"/>
       <c r="BU27" s="2"/>
-      <c r="BV27" s="40">
+      <c r="BV27" s="26">
         <v>3</v>
       </c>
-      <c r="BW27" s="40">
+      <c r="BW27" s="26">
         <v>3</v>
       </c>
       <c r="BX27" s="1"/>
@@ -5945,21 +5940,21 @@
       <c r="BZ27" s="1"/>
       <c r="CA27" s="3"/>
       <c r="CB27" s="2"/>
-      <c r="CC27" s="40">
+      <c r="CC27" s="26">
         <v>3</v>
       </c>
-      <c r="CD27" s="40">
+      <c r="CD27" s="26">
         <v>3</v>
       </c>
-      <c r="CE27" s="34"/>
-      <c r="CF27" s="34"/>
+      <c r="CE27" s="1"/>
+      <c r="CF27" s="1"/>
       <c r="CG27" s="1"/>
       <c r="CH27" s="3"/>
       <c r="CI27" s="2"/>
-      <c r="CJ27" s="40">
+      <c r="CJ27" s="26">
         <v>3</v>
       </c>
-      <c r="CK27" s="40">
+      <c r="CK27" s="26">
         <v>3</v>
       </c>
       <c r="CL27" s="1"/>
@@ -5967,10 +5962,10 @@
       <c r="CN27" s="1"/>
       <c r="CO27" s="3"/>
       <c r="CP27" s="2"/>
-      <c r="CQ27" s="40">
+      <c r="CQ27" s="26">
         <v>3</v>
       </c>
-      <c r="CR27" s="40">
+      <c r="CR27" s="26">
         <v>3</v>
       </c>
       <c r="CS27" s="1"/>
@@ -5978,10 +5973,10 @@
       <c r="CU27" s="1"/>
       <c r="CV27" s="3"/>
       <c r="CW27" s="2"/>
-      <c r="CX27" s="40">
+      <c r="CX27" s="26">
         <v>3</v>
       </c>
-      <c r="CY27" s="40">
+      <c r="CY27" s="26">
         <v>3</v>
       </c>
       <c r="CZ27" s="1"/>
@@ -5995,20 +5990,20 @@
       <c r="DH27" s="1"/>
       <c r="DI27" s="1"/>
       <c r="DJ27" s="3"/>
-      <c r="DK27" s="48"/>
-      <c r="DL27" s="49"/>
-      <c r="DM27" s="49"/>
-      <c r="DN27" s="49"/>
-      <c r="DO27" s="49"/>
-      <c r="DP27" s="49"/>
-      <c r="DQ27" s="50"/>
-      <c r="DR27" s="48"/>
-      <c r="DS27" s="49"/>
-      <c r="DT27" s="49"/>
-      <c r="DU27" s="49"/>
-      <c r="DV27" s="49"/>
-      <c r="DW27" s="49"/>
-      <c r="DX27" s="50"/>
+      <c r="DK27" s="60"/>
+      <c r="DL27" s="61"/>
+      <c r="DM27" s="61"/>
+      <c r="DN27" s="61"/>
+      <c r="DO27" s="61"/>
+      <c r="DP27" s="61"/>
+      <c r="DQ27" s="62"/>
+      <c r="DR27" s="60"/>
+      <c r="DS27" s="61"/>
+      <c r="DT27" s="61"/>
+      <c r="DU27" s="61"/>
+      <c r="DV27" s="61"/>
+      <c r="DW27" s="61"/>
+      <c r="DX27" s="62"/>
       <c r="DY27" s="2"/>
       <c r="DZ27" s="1"/>
       <c r="EA27" s="1"/>
@@ -6025,8 +6020,8 @@
       <c r="EL27" s="3"/>
     </row>
     <row r="28" spans="1:142" ht="15" thickBot="1">
-      <c r="A28" s="69"/>
-      <c r="B28" s="36" t="s">
+      <c r="A28" s="37"/>
+      <c r="B28" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="2"/>
@@ -6064,13 +6059,13 @@
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="3"/>
-      <c r="AL28" s="57"/>
-      <c r="AM28" s="58"/>
-      <c r="AN28" s="58"/>
-      <c r="AO28" s="58"/>
-      <c r="AP28" s="58"/>
-      <c r="AQ28" s="58"/>
-      <c r="AR28" s="59"/>
+      <c r="AL28" s="52"/>
+      <c r="AM28" s="53"/>
+      <c r="AN28" s="53"/>
+      <c r="AO28" s="53"/>
+      <c r="AP28" s="53"/>
+      <c r="AQ28" s="53"/>
+      <c r="AR28" s="54"/>
       <c r="AS28" s="2"/>
       <c r="AT28" s="1"/>
       <c r="AU28" s="1"/>
@@ -6109,8 +6104,8 @@
       <c r="CB28" s="2"/>
       <c r="CC28" s="1"/>
       <c r="CD28" s="1"/>
-      <c r="CE28" s="34"/>
-      <c r="CF28" s="34"/>
+      <c r="CE28" s="1"/>
+      <c r="CF28" s="1"/>
       <c r="CG28" s="1"/>
       <c r="CH28" s="3"/>
       <c r="CI28" s="2"/>
@@ -6141,20 +6136,20 @@
       <c r="DH28" s="1"/>
       <c r="DI28" s="1"/>
       <c r="DJ28" s="3"/>
-      <c r="DK28" s="48"/>
-      <c r="DL28" s="49"/>
-      <c r="DM28" s="49"/>
-      <c r="DN28" s="49"/>
-      <c r="DO28" s="49"/>
-      <c r="DP28" s="49"/>
-      <c r="DQ28" s="50"/>
-      <c r="DR28" s="48"/>
-      <c r="DS28" s="49"/>
-      <c r="DT28" s="49"/>
-      <c r="DU28" s="49"/>
-      <c r="DV28" s="49"/>
-      <c r="DW28" s="49"/>
-      <c r="DX28" s="50"/>
+      <c r="DK28" s="60"/>
+      <c r="DL28" s="61"/>
+      <c r="DM28" s="61"/>
+      <c r="DN28" s="61"/>
+      <c r="DO28" s="61"/>
+      <c r="DP28" s="61"/>
+      <c r="DQ28" s="62"/>
+      <c r="DR28" s="60"/>
+      <c r="DS28" s="61"/>
+      <c r="DT28" s="61"/>
+      <c r="DU28" s="61"/>
+      <c r="DV28" s="61"/>
+      <c r="DW28" s="61"/>
+      <c r="DX28" s="62"/>
       <c r="DY28" s="2"/>
       <c r="DZ28" s="1"/>
       <c r="EA28" s="1"/>
@@ -6171,10 +6166,10 @@
       <c r="EL28" s="3"/>
     </row>
     <row r="29" spans="1:142" ht="15" thickBot="1">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="2"/>
@@ -6212,13 +6207,13 @@
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="3"/>
-      <c r="AL29" s="57"/>
-      <c r="AM29" s="58"/>
-      <c r="AN29" s="58"/>
-      <c r="AO29" s="58"/>
-      <c r="AP29" s="58"/>
-      <c r="AQ29" s="58"/>
-      <c r="AR29" s="59"/>
+      <c r="AL29" s="52"/>
+      <c r="AM29" s="53"/>
+      <c r="AN29" s="53"/>
+      <c r="AO29" s="53"/>
+      <c r="AP29" s="53"/>
+      <c r="AQ29" s="53"/>
+      <c r="AR29" s="54"/>
       <c r="AS29" s="2"/>
       <c r="AT29" s="1"/>
       <c r="AU29" s="1"/>
@@ -6284,31 +6279,31 @@
       <c r="DC29" s="3"/>
       <c r="DD29" s="2"/>
       <c r="DE29" s="1"/>
-      <c r="DF29" s="40">
+      <c r="DF29" s="26">
         <v>1</v>
       </c>
-      <c r="DG29" s="40">
+      <c r="DG29" s="26">
         <v>1</v>
       </c>
-      <c r="DH29" s="40">
+      <c r="DH29" s="26">
         <v>1</v>
       </c>
-      <c r="DI29" s="34"/>
+      <c r="DI29" s="1"/>
       <c r="DJ29" s="3"/>
-      <c r="DK29" s="48"/>
-      <c r="DL29" s="49"/>
-      <c r="DM29" s="49"/>
-      <c r="DN29" s="49"/>
-      <c r="DO29" s="49"/>
-      <c r="DP29" s="49"/>
-      <c r="DQ29" s="50"/>
-      <c r="DR29" s="48"/>
-      <c r="DS29" s="49"/>
-      <c r="DT29" s="49"/>
-      <c r="DU29" s="49"/>
-      <c r="DV29" s="49"/>
-      <c r="DW29" s="49"/>
-      <c r="DX29" s="50"/>
+      <c r="DK29" s="60"/>
+      <c r="DL29" s="61"/>
+      <c r="DM29" s="61"/>
+      <c r="DN29" s="61"/>
+      <c r="DO29" s="61"/>
+      <c r="DP29" s="61"/>
+      <c r="DQ29" s="62"/>
+      <c r="DR29" s="60"/>
+      <c r="DS29" s="61"/>
+      <c r="DT29" s="61"/>
+      <c r="DU29" s="61"/>
+      <c r="DV29" s="61"/>
+      <c r="DW29" s="61"/>
+      <c r="DX29" s="62"/>
       <c r="DY29" s="2"/>
       <c r="DZ29" s="1"/>
       <c r="EA29" s="1"/>
@@ -6325,8 +6320,8 @@
       <c r="EL29" s="3"/>
     </row>
     <row r="30" spans="1:142" ht="15" thickBot="1">
-      <c r="A30" s="72"/>
-      <c r="B30" s="36" t="s">
+      <c r="A30" s="38"/>
+      <c r="B30" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="2"/>
@@ -6364,13 +6359,13 @@
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="3"/>
-      <c r="AL30" s="57"/>
-      <c r="AM30" s="58"/>
-      <c r="AN30" s="58"/>
-      <c r="AO30" s="58"/>
-      <c r="AP30" s="58"/>
-      <c r="AQ30" s="58"/>
-      <c r="AR30" s="59"/>
+      <c r="AL30" s="52"/>
+      <c r="AM30" s="53"/>
+      <c r="AN30" s="53"/>
+      <c r="AO30" s="53"/>
+      <c r="AP30" s="53"/>
+      <c r="AQ30" s="53"/>
+      <c r="AR30" s="54"/>
       <c r="AS30" s="2"/>
       <c r="AT30" s="1"/>
       <c r="AU30" s="1"/>
@@ -6441,20 +6436,20 @@
       <c r="DH30" s="1"/>
       <c r="DI30" s="1"/>
       <c r="DJ30" s="3"/>
-      <c r="DK30" s="48"/>
-      <c r="DL30" s="49"/>
-      <c r="DM30" s="49"/>
-      <c r="DN30" s="49"/>
-      <c r="DO30" s="49"/>
-      <c r="DP30" s="49"/>
-      <c r="DQ30" s="50"/>
-      <c r="DR30" s="48"/>
-      <c r="DS30" s="49"/>
-      <c r="DT30" s="49"/>
-      <c r="DU30" s="49"/>
-      <c r="DV30" s="49"/>
-      <c r="DW30" s="49"/>
-      <c r="DX30" s="50"/>
+      <c r="DK30" s="60"/>
+      <c r="DL30" s="61"/>
+      <c r="DM30" s="61"/>
+      <c r="DN30" s="61"/>
+      <c r="DO30" s="61"/>
+      <c r="DP30" s="61"/>
+      <c r="DQ30" s="62"/>
+      <c r="DR30" s="60"/>
+      <c r="DS30" s="61"/>
+      <c r="DT30" s="61"/>
+      <c r="DU30" s="61"/>
+      <c r="DV30" s="61"/>
+      <c r="DW30" s="61"/>
+      <c r="DX30" s="62"/>
       <c r="DY30" s="2"/>
       <c r="DZ30" s="1"/>
       <c r="EA30" s="1"/>
@@ -6471,10 +6466,10 @@
       <c r="EL30" s="3"/>
     </row>
     <row r="31" spans="1:142" ht="15" thickBot="1">
-      <c r="A31" s="68" t="s">
+      <c r="A31" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="2"/>
@@ -6512,13 +6507,13 @@
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="3"/>
-      <c r="AL31" s="57"/>
-      <c r="AM31" s="58"/>
-      <c r="AN31" s="58"/>
-      <c r="AO31" s="58"/>
-      <c r="AP31" s="58"/>
-      <c r="AQ31" s="58"/>
-      <c r="AR31" s="59"/>
+      <c r="AL31" s="52"/>
+      <c r="AM31" s="53"/>
+      <c r="AN31" s="53"/>
+      <c r="AO31" s="53"/>
+      <c r="AP31" s="53"/>
+      <c r="AQ31" s="53"/>
+      <c r="AR31" s="54"/>
       <c r="AS31" s="2"/>
       <c r="AT31" s="1"/>
       <c r="AU31" s="1"/>
@@ -6589,42 +6584,42 @@
       <c r="DH31" s="1"/>
       <c r="DI31" s="1"/>
       <c r="DJ31" s="3"/>
-      <c r="DK31" s="48"/>
-      <c r="DL31" s="49"/>
-      <c r="DM31" s="49"/>
-      <c r="DN31" s="49"/>
-      <c r="DO31" s="49"/>
-      <c r="DP31" s="49"/>
-      <c r="DQ31" s="50"/>
-      <c r="DR31" s="48"/>
-      <c r="DS31" s="49"/>
-      <c r="DT31" s="49"/>
-      <c r="DU31" s="49"/>
-      <c r="DV31" s="49"/>
-      <c r="DW31" s="49"/>
-      <c r="DX31" s="50"/>
-      <c r="DY31" s="44">
+      <c r="DK31" s="60"/>
+      <c r="DL31" s="61"/>
+      <c r="DM31" s="61"/>
+      <c r="DN31" s="61"/>
+      <c r="DO31" s="61"/>
+      <c r="DP31" s="61"/>
+      <c r="DQ31" s="62"/>
+      <c r="DR31" s="60"/>
+      <c r="DS31" s="61"/>
+      <c r="DT31" s="61"/>
+      <c r="DU31" s="61"/>
+      <c r="DV31" s="61"/>
+      <c r="DW31" s="61"/>
+      <c r="DX31" s="62"/>
+      <c r="DY31" s="28">
         <v>1</v>
       </c>
-      <c r="DZ31" s="40">
+      <c r="DZ31" s="26">
         <v>1</v>
       </c>
-      <c r="EA31" s="40">
+      <c r="EA31" s="26">
         <v>1</v>
       </c>
-      <c r="EB31" s="40">
+      <c r="EB31" s="26">
         <v>1</v>
       </c>
-      <c r="EC31" s="40">
+      <c r="EC31" s="26">
         <v>1</v>
       </c>
-      <c r="ED31" s="40">
+      <c r="ED31" s="26">
         <v>1</v>
       </c>
-      <c r="EE31" s="45">
+      <c r="EE31" s="29">
         <v>1</v>
       </c>
-      <c r="EF31" s="44">
+      <c r="EF31" s="28">
         <v>0.5</v>
       </c>
       <c r="EG31" s="1"/>
@@ -6635,8 +6630,8 @@
       <c r="EL31" s="3"/>
     </row>
     <row r="32" spans="1:142" ht="15" thickBot="1">
-      <c r="A32" s="69"/>
-      <c r="B32" s="36" t="s">
+      <c r="A32" s="37"/>
+      <c r="B32" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="2"/>
@@ -6674,13 +6669,13 @@
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
       <c r="AK32" s="3"/>
-      <c r="AL32" s="57"/>
-      <c r="AM32" s="58"/>
-      <c r="AN32" s="58"/>
-      <c r="AO32" s="58"/>
-      <c r="AP32" s="58"/>
-      <c r="AQ32" s="58"/>
-      <c r="AR32" s="59"/>
+      <c r="AL32" s="52"/>
+      <c r="AM32" s="53"/>
+      <c r="AN32" s="53"/>
+      <c r="AO32" s="53"/>
+      <c r="AP32" s="53"/>
+      <c r="AQ32" s="53"/>
+      <c r="AR32" s="54"/>
       <c r="AS32" s="2"/>
       <c r="AT32" s="1"/>
       <c r="AU32" s="1"/>
@@ -6751,20 +6746,20 @@
       <c r="DH32" s="1"/>
       <c r="DI32" s="1"/>
       <c r="DJ32" s="3"/>
-      <c r="DK32" s="48"/>
-      <c r="DL32" s="49"/>
-      <c r="DM32" s="49"/>
-      <c r="DN32" s="49"/>
-      <c r="DO32" s="49"/>
-      <c r="DP32" s="49"/>
-      <c r="DQ32" s="50"/>
-      <c r="DR32" s="48"/>
-      <c r="DS32" s="49"/>
-      <c r="DT32" s="49"/>
-      <c r="DU32" s="49"/>
-      <c r="DV32" s="49"/>
-      <c r="DW32" s="49"/>
-      <c r="DX32" s="50"/>
+      <c r="DK32" s="60"/>
+      <c r="DL32" s="61"/>
+      <c r="DM32" s="61"/>
+      <c r="DN32" s="61"/>
+      <c r="DO32" s="61"/>
+      <c r="DP32" s="61"/>
+      <c r="DQ32" s="62"/>
+      <c r="DR32" s="60"/>
+      <c r="DS32" s="61"/>
+      <c r="DT32" s="61"/>
+      <c r="DU32" s="61"/>
+      <c r="DV32" s="61"/>
+      <c r="DW32" s="61"/>
+      <c r="DX32" s="62"/>
       <c r="DY32" s="2"/>
       <c r="DZ32" s="1"/>
       <c r="EA32" s="1"/>
@@ -6781,10 +6776,10 @@
       <c r="EL32" s="3"/>
     </row>
     <row r="33" spans="1:142" ht="15" thickBot="1">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="2"/>
@@ -6822,13 +6817,13 @@
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>
       <c r="AK33" s="3"/>
-      <c r="AL33" s="57"/>
-      <c r="AM33" s="58"/>
-      <c r="AN33" s="58"/>
-      <c r="AO33" s="58"/>
-      <c r="AP33" s="58"/>
-      <c r="AQ33" s="58"/>
-      <c r="AR33" s="59"/>
+      <c r="AL33" s="52"/>
+      <c r="AM33" s="53"/>
+      <c r="AN33" s="53"/>
+      <c r="AO33" s="53"/>
+      <c r="AP33" s="53"/>
+      <c r="AQ33" s="53"/>
+      <c r="AR33" s="54"/>
       <c r="AS33" s="2"/>
       <c r="AT33" s="1"/>
       <c r="AU33" s="1"/>
@@ -6899,20 +6894,20 @@
       <c r="DH33" s="1"/>
       <c r="DI33" s="1"/>
       <c r="DJ33" s="3"/>
-      <c r="DK33" s="48"/>
-      <c r="DL33" s="49"/>
-      <c r="DM33" s="49"/>
-      <c r="DN33" s="49"/>
-      <c r="DO33" s="49"/>
-      <c r="DP33" s="49"/>
-      <c r="DQ33" s="50"/>
-      <c r="DR33" s="48"/>
-      <c r="DS33" s="49"/>
-      <c r="DT33" s="49"/>
-      <c r="DU33" s="49"/>
-      <c r="DV33" s="49"/>
-      <c r="DW33" s="49"/>
-      <c r="DX33" s="50"/>
+      <c r="DK33" s="60"/>
+      <c r="DL33" s="61"/>
+      <c r="DM33" s="61"/>
+      <c r="DN33" s="61"/>
+      <c r="DO33" s="61"/>
+      <c r="DP33" s="61"/>
+      <c r="DQ33" s="62"/>
+      <c r="DR33" s="60"/>
+      <c r="DS33" s="61"/>
+      <c r="DT33" s="61"/>
+      <c r="DU33" s="61"/>
+      <c r="DV33" s="61"/>
+      <c r="DW33" s="61"/>
+      <c r="DX33" s="62"/>
       <c r="DY33" s="2"/>
       <c r="DZ33" s="1"/>
       <c r="EA33" s="1"/>
@@ -6921,7 +6916,7 @@
       <c r="ED33" s="1"/>
       <c r="EE33" s="3"/>
       <c r="EF33" s="2"/>
-      <c r="EG33" s="40">
+      <c r="EG33" s="26">
         <v>0.5</v>
       </c>
       <c r="EH33" s="1"/>
@@ -6931,8 +6926,8 @@
       <c r="EL33" s="3"/>
     </row>
     <row r="34" spans="1:142" ht="15" thickBot="1">
-      <c r="A34" s="72"/>
-      <c r="B34" s="36" t="s">
+      <c r="A34" s="38"/>
+      <c r="B34" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="2"/>
@@ -6970,13 +6965,13 @@
       <c r="AI34" s="1"/>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="3"/>
-      <c r="AL34" s="57"/>
-      <c r="AM34" s="58"/>
-      <c r="AN34" s="58"/>
-      <c r="AO34" s="58"/>
-      <c r="AP34" s="58"/>
-      <c r="AQ34" s="58"/>
-      <c r="AR34" s="59"/>
+      <c r="AL34" s="52"/>
+      <c r="AM34" s="53"/>
+      <c r="AN34" s="53"/>
+      <c r="AO34" s="53"/>
+      <c r="AP34" s="53"/>
+      <c r="AQ34" s="53"/>
+      <c r="AR34" s="54"/>
       <c r="AS34" s="2"/>
       <c r="AT34" s="1"/>
       <c r="AU34" s="1"/>
@@ -7047,20 +7042,20 @@
       <c r="DH34" s="1"/>
       <c r="DI34" s="1"/>
       <c r="DJ34" s="3"/>
-      <c r="DK34" s="48"/>
-      <c r="DL34" s="49"/>
-      <c r="DM34" s="49"/>
-      <c r="DN34" s="49"/>
-      <c r="DO34" s="49"/>
-      <c r="DP34" s="49"/>
-      <c r="DQ34" s="50"/>
-      <c r="DR34" s="48"/>
-      <c r="DS34" s="49"/>
-      <c r="DT34" s="49"/>
-      <c r="DU34" s="49"/>
-      <c r="DV34" s="49"/>
-      <c r="DW34" s="49"/>
-      <c r="DX34" s="50"/>
+      <c r="DK34" s="60"/>
+      <c r="DL34" s="61"/>
+      <c r="DM34" s="61"/>
+      <c r="DN34" s="61"/>
+      <c r="DO34" s="61"/>
+      <c r="DP34" s="61"/>
+      <c r="DQ34" s="62"/>
+      <c r="DR34" s="60"/>
+      <c r="DS34" s="61"/>
+      <c r="DT34" s="61"/>
+      <c r="DU34" s="61"/>
+      <c r="DV34" s="61"/>
+      <c r="DW34" s="61"/>
+      <c r="DX34" s="62"/>
       <c r="DY34" s="2"/>
       <c r="DZ34" s="1"/>
       <c r="EA34" s="1"/>
@@ -7077,8 +7072,8 @@
       <c r="EL34" s="3"/>
     </row>
     <row r="35" spans="1:142" ht="15" thickBot="1">
-      <c r="A35" s="19"/>
-      <c r="B35" s="37" t="s">
+      <c r="A35" s="32"/>
+      <c r="B35" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="2"/>
@@ -7116,13 +7111,13 @@
       <c r="AI35" s="1"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="3"/>
-      <c r="AL35" s="57"/>
-      <c r="AM35" s="58"/>
-      <c r="AN35" s="58"/>
-      <c r="AO35" s="58"/>
-      <c r="AP35" s="58"/>
-      <c r="AQ35" s="58"/>
-      <c r="AR35" s="59"/>
+      <c r="AL35" s="52"/>
+      <c r="AM35" s="53"/>
+      <c r="AN35" s="53"/>
+      <c r="AO35" s="53"/>
+      <c r="AP35" s="53"/>
+      <c r="AQ35" s="53"/>
+      <c r="AR35" s="54"/>
       <c r="AS35" s="2"/>
       <c r="AT35" s="1"/>
       <c r="AU35" s="1"/>
@@ -7193,20 +7188,20 @@
       <c r="DH35" s="1"/>
       <c r="DI35" s="1"/>
       <c r="DJ35" s="3"/>
-      <c r="DK35" s="48"/>
-      <c r="DL35" s="49"/>
-      <c r="DM35" s="49"/>
-      <c r="DN35" s="49"/>
-      <c r="DO35" s="49"/>
-      <c r="DP35" s="49"/>
-      <c r="DQ35" s="50"/>
-      <c r="DR35" s="48"/>
-      <c r="DS35" s="49"/>
-      <c r="DT35" s="49"/>
-      <c r="DU35" s="49"/>
-      <c r="DV35" s="49"/>
-      <c r="DW35" s="49"/>
-      <c r="DX35" s="50"/>
+      <c r="DK35" s="60"/>
+      <c r="DL35" s="61"/>
+      <c r="DM35" s="61"/>
+      <c r="DN35" s="61"/>
+      <c r="DO35" s="61"/>
+      <c r="DP35" s="61"/>
+      <c r="DQ35" s="62"/>
+      <c r="DR35" s="60"/>
+      <c r="DS35" s="61"/>
+      <c r="DT35" s="61"/>
+      <c r="DU35" s="61"/>
+      <c r="DV35" s="61"/>
+      <c r="DW35" s="61"/>
+      <c r="DX35" s="62"/>
       <c r="DY35" s="2"/>
       <c r="DZ35" s="1"/>
       <c r="EA35" s="1"/>
@@ -7223,8 +7218,8 @@
       <c r="EL35" s="3"/>
     </row>
     <row r="36" spans="1:142" ht="15" thickBot="1">
-      <c r="A36" s="20"/>
-      <c r="B36" s="36" t="s">
+      <c r="A36" s="33"/>
+      <c r="B36" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="2"/>
@@ -7262,13 +7257,13 @@
       <c r="AI36" s="1"/>
       <c r="AJ36" s="1"/>
       <c r="AK36" s="3"/>
-      <c r="AL36" s="57"/>
-      <c r="AM36" s="58"/>
-      <c r="AN36" s="58"/>
-      <c r="AO36" s="58"/>
-      <c r="AP36" s="58"/>
-      <c r="AQ36" s="58"/>
-      <c r="AR36" s="59"/>
+      <c r="AL36" s="52"/>
+      <c r="AM36" s="53"/>
+      <c r="AN36" s="53"/>
+      <c r="AO36" s="53"/>
+      <c r="AP36" s="53"/>
+      <c r="AQ36" s="53"/>
+      <c r="AR36" s="54"/>
       <c r="AS36" s="2"/>
       <c r="AT36" s="1"/>
       <c r="AU36" s="1"/>
@@ -7339,20 +7334,20 @@
       <c r="DH36" s="1"/>
       <c r="DI36" s="1"/>
       <c r="DJ36" s="3"/>
-      <c r="DK36" s="48"/>
-      <c r="DL36" s="49"/>
-      <c r="DM36" s="49"/>
-      <c r="DN36" s="49"/>
-      <c r="DO36" s="49"/>
-      <c r="DP36" s="49"/>
-      <c r="DQ36" s="50"/>
-      <c r="DR36" s="48"/>
-      <c r="DS36" s="49"/>
-      <c r="DT36" s="49"/>
-      <c r="DU36" s="49"/>
-      <c r="DV36" s="49"/>
-      <c r="DW36" s="49"/>
-      <c r="DX36" s="50"/>
+      <c r="DK36" s="60"/>
+      <c r="DL36" s="61"/>
+      <c r="DM36" s="61"/>
+      <c r="DN36" s="61"/>
+      <c r="DO36" s="61"/>
+      <c r="DP36" s="61"/>
+      <c r="DQ36" s="62"/>
+      <c r="DR36" s="60"/>
+      <c r="DS36" s="61"/>
+      <c r="DT36" s="61"/>
+      <c r="DU36" s="61"/>
+      <c r="DV36" s="61"/>
+      <c r="DW36" s="61"/>
+      <c r="DX36" s="62"/>
       <c r="DY36" s="2"/>
       <c r="DZ36" s="1"/>
       <c r="EA36" s="1"/>
@@ -7369,8 +7364,8 @@
       <c r="EL36" s="3"/>
     </row>
     <row r="37" spans="1:142" ht="15" thickBot="1">
-      <c r="A37" s="19"/>
-      <c r="B37" s="37" t="s">
+      <c r="A37" s="32"/>
+      <c r="B37" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C37" s="2"/>
@@ -7408,13 +7403,13 @@
       <c r="AI37" s="1"/>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="3"/>
-      <c r="AL37" s="57"/>
-      <c r="AM37" s="58"/>
-      <c r="AN37" s="58"/>
-      <c r="AO37" s="58"/>
-      <c r="AP37" s="58"/>
-      <c r="AQ37" s="58"/>
-      <c r="AR37" s="59"/>
+      <c r="AL37" s="52"/>
+      <c r="AM37" s="53"/>
+      <c r="AN37" s="53"/>
+      <c r="AO37" s="53"/>
+      <c r="AP37" s="53"/>
+      <c r="AQ37" s="53"/>
+      <c r="AR37" s="54"/>
       <c r="AS37" s="2"/>
       <c r="AT37" s="1"/>
       <c r="AU37" s="1"/>
@@ -7485,20 +7480,20 @@
       <c r="DH37" s="1"/>
       <c r="DI37" s="1"/>
       <c r="DJ37" s="3"/>
-      <c r="DK37" s="48"/>
-      <c r="DL37" s="49"/>
-      <c r="DM37" s="49"/>
-      <c r="DN37" s="49"/>
-      <c r="DO37" s="49"/>
-      <c r="DP37" s="49"/>
-      <c r="DQ37" s="50"/>
-      <c r="DR37" s="48"/>
-      <c r="DS37" s="49"/>
-      <c r="DT37" s="49"/>
-      <c r="DU37" s="49"/>
-      <c r="DV37" s="49"/>
-      <c r="DW37" s="49"/>
-      <c r="DX37" s="50"/>
+      <c r="DK37" s="60"/>
+      <c r="DL37" s="61"/>
+      <c r="DM37" s="61"/>
+      <c r="DN37" s="61"/>
+      <c r="DO37" s="61"/>
+      <c r="DP37" s="61"/>
+      <c r="DQ37" s="62"/>
+      <c r="DR37" s="60"/>
+      <c r="DS37" s="61"/>
+      <c r="DT37" s="61"/>
+      <c r="DU37" s="61"/>
+      <c r="DV37" s="61"/>
+      <c r="DW37" s="61"/>
+      <c r="DX37" s="62"/>
       <c r="DY37" s="2"/>
       <c r="DZ37" s="1"/>
       <c r="EA37" s="1"/>
@@ -7515,8 +7510,8 @@
       <c r="EL37" s="3"/>
     </row>
     <row r="38" spans="1:142" ht="15" thickBot="1">
-      <c r="A38" s="20"/>
-      <c r="B38" s="36" t="s">
+      <c r="A38" s="33"/>
+      <c r="B38" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C38" s="2"/>
@@ -7554,13 +7549,13 @@
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="3"/>
-      <c r="AL38" s="57"/>
-      <c r="AM38" s="58"/>
-      <c r="AN38" s="58"/>
-      <c r="AO38" s="58"/>
-      <c r="AP38" s="58"/>
-      <c r="AQ38" s="58"/>
-      <c r="AR38" s="59"/>
+      <c r="AL38" s="52"/>
+      <c r="AM38" s="53"/>
+      <c r="AN38" s="53"/>
+      <c r="AO38" s="53"/>
+      <c r="AP38" s="53"/>
+      <c r="AQ38" s="53"/>
+      <c r="AR38" s="54"/>
       <c r="AS38" s="2"/>
       <c r="AT38" s="1"/>
       <c r="AU38" s="1"/>
@@ -7631,20 +7626,20 @@
       <c r="DH38" s="1"/>
       <c r="DI38" s="1"/>
       <c r="DJ38" s="3"/>
-      <c r="DK38" s="48"/>
-      <c r="DL38" s="49"/>
-      <c r="DM38" s="49"/>
-      <c r="DN38" s="49"/>
-      <c r="DO38" s="49"/>
-      <c r="DP38" s="49"/>
-      <c r="DQ38" s="50"/>
-      <c r="DR38" s="48"/>
-      <c r="DS38" s="49"/>
-      <c r="DT38" s="49"/>
-      <c r="DU38" s="49"/>
-      <c r="DV38" s="49"/>
-      <c r="DW38" s="49"/>
-      <c r="DX38" s="50"/>
+      <c r="DK38" s="60"/>
+      <c r="DL38" s="61"/>
+      <c r="DM38" s="61"/>
+      <c r="DN38" s="61"/>
+      <c r="DO38" s="61"/>
+      <c r="DP38" s="61"/>
+      <c r="DQ38" s="62"/>
+      <c r="DR38" s="60"/>
+      <c r="DS38" s="61"/>
+      <c r="DT38" s="61"/>
+      <c r="DU38" s="61"/>
+      <c r="DV38" s="61"/>
+      <c r="DW38" s="61"/>
+      <c r="DX38" s="62"/>
       <c r="DY38" s="2"/>
       <c r="DZ38" s="1"/>
       <c r="EA38" s="1"/>
@@ -7661,8 +7656,8 @@
       <c r="EL38" s="3"/>
     </row>
     <row r="39" spans="1:142" ht="15" thickBot="1">
-      <c r="A39" s="19"/>
-      <c r="B39" s="37" t="s">
+      <c r="A39" s="32"/>
+      <c r="B39" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="2"/>
@@ -7700,13 +7695,13 @@
       <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
       <c r="AK39" s="3"/>
-      <c r="AL39" s="57"/>
-      <c r="AM39" s="58"/>
-      <c r="AN39" s="58"/>
-      <c r="AO39" s="58"/>
-      <c r="AP39" s="58"/>
-      <c r="AQ39" s="58"/>
-      <c r="AR39" s="59"/>
+      <c r="AL39" s="52"/>
+      <c r="AM39" s="53"/>
+      <c r="AN39" s="53"/>
+      <c r="AO39" s="53"/>
+      <c r="AP39" s="53"/>
+      <c r="AQ39" s="53"/>
+      <c r="AR39" s="54"/>
       <c r="AS39" s="2"/>
       <c r="AT39" s="1"/>
       <c r="AU39" s="1"/>
@@ -7777,20 +7772,20 @@
       <c r="DH39" s="1"/>
       <c r="DI39" s="1"/>
       <c r="DJ39" s="3"/>
-      <c r="DK39" s="48"/>
-      <c r="DL39" s="49"/>
-      <c r="DM39" s="49"/>
-      <c r="DN39" s="49"/>
-      <c r="DO39" s="49"/>
-      <c r="DP39" s="49"/>
-      <c r="DQ39" s="50"/>
-      <c r="DR39" s="48"/>
-      <c r="DS39" s="49"/>
-      <c r="DT39" s="49"/>
-      <c r="DU39" s="49"/>
-      <c r="DV39" s="49"/>
-      <c r="DW39" s="49"/>
-      <c r="DX39" s="50"/>
+      <c r="DK39" s="60"/>
+      <c r="DL39" s="61"/>
+      <c r="DM39" s="61"/>
+      <c r="DN39" s="61"/>
+      <c r="DO39" s="61"/>
+      <c r="DP39" s="61"/>
+      <c r="DQ39" s="62"/>
+      <c r="DR39" s="60"/>
+      <c r="DS39" s="61"/>
+      <c r="DT39" s="61"/>
+      <c r="DU39" s="61"/>
+      <c r="DV39" s="61"/>
+      <c r="DW39" s="61"/>
+      <c r="DX39" s="62"/>
       <c r="DY39" s="2"/>
       <c r="DZ39" s="1"/>
       <c r="EA39" s="1"/>
@@ -7807,8 +7802,8 @@
       <c r="EL39" s="3"/>
     </row>
     <row r="40" spans="1:142" ht="15" thickBot="1">
-      <c r="A40" s="20"/>
-      <c r="B40" s="36" t="s">
+      <c r="A40" s="33"/>
+      <c r="B40" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C40" s="2"/>
@@ -7846,13 +7841,13 @@
       <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
       <c r="AK40" s="3"/>
-      <c r="AL40" s="57"/>
-      <c r="AM40" s="58"/>
-      <c r="AN40" s="58"/>
-      <c r="AO40" s="58"/>
-      <c r="AP40" s="58"/>
-      <c r="AQ40" s="58"/>
-      <c r="AR40" s="59"/>
+      <c r="AL40" s="52"/>
+      <c r="AM40" s="53"/>
+      <c r="AN40" s="53"/>
+      <c r="AO40" s="53"/>
+      <c r="AP40" s="53"/>
+      <c r="AQ40" s="53"/>
+      <c r="AR40" s="54"/>
       <c r="AS40" s="2"/>
       <c r="AT40" s="1"/>
       <c r="AU40" s="1"/>
@@ -7923,20 +7918,20 @@
       <c r="DH40" s="1"/>
       <c r="DI40" s="1"/>
       <c r="DJ40" s="3"/>
-      <c r="DK40" s="48"/>
-      <c r="DL40" s="49"/>
-      <c r="DM40" s="49"/>
-      <c r="DN40" s="49"/>
-      <c r="DO40" s="49"/>
-      <c r="DP40" s="49"/>
-      <c r="DQ40" s="50"/>
-      <c r="DR40" s="48"/>
-      <c r="DS40" s="49"/>
-      <c r="DT40" s="49"/>
-      <c r="DU40" s="49"/>
-      <c r="DV40" s="49"/>
-      <c r="DW40" s="49"/>
-      <c r="DX40" s="50"/>
+      <c r="DK40" s="60"/>
+      <c r="DL40" s="61"/>
+      <c r="DM40" s="61"/>
+      <c r="DN40" s="61"/>
+      <c r="DO40" s="61"/>
+      <c r="DP40" s="61"/>
+      <c r="DQ40" s="62"/>
+      <c r="DR40" s="60"/>
+      <c r="DS40" s="61"/>
+      <c r="DT40" s="61"/>
+      <c r="DU40" s="61"/>
+      <c r="DV40" s="61"/>
+      <c r="DW40" s="61"/>
+      <c r="DX40" s="62"/>
       <c r="DY40" s="2"/>
       <c r="DZ40" s="1"/>
       <c r="EA40" s="1"/>
@@ -7953,10 +7948,10 @@
       <c r="EL40" s="3"/>
     </row>
     <row r="41" spans="1:142" ht="15" thickBot="1">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C41" s="2"/>
@@ -7994,13 +7989,13 @@
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="3"/>
-      <c r="AL41" s="57"/>
-      <c r="AM41" s="58"/>
-      <c r="AN41" s="58"/>
-      <c r="AO41" s="58"/>
-      <c r="AP41" s="58"/>
-      <c r="AQ41" s="58"/>
-      <c r="AR41" s="59"/>
+      <c r="AL41" s="52"/>
+      <c r="AM41" s="53"/>
+      <c r="AN41" s="53"/>
+      <c r="AO41" s="53"/>
+      <c r="AP41" s="53"/>
+      <c r="AQ41" s="53"/>
+      <c r="AR41" s="54"/>
       <c r="AS41" s="2"/>
       <c r="AT41" s="1"/>
       <c r="AU41" s="1"/>
@@ -8071,20 +8066,20 @@
       <c r="DH41" s="1"/>
       <c r="DI41" s="1"/>
       <c r="DJ41" s="3"/>
-      <c r="DK41" s="48"/>
-      <c r="DL41" s="49"/>
-      <c r="DM41" s="49"/>
-      <c r="DN41" s="49"/>
-      <c r="DO41" s="49"/>
-      <c r="DP41" s="49"/>
-      <c r="DQ41" s="50"/>
-      <c r="DR41" s="48"/>
-      <c r="DS41" s="49"/>
-      <c r="DT41" s="49"/>
-      <c r="DU41" s="49"/>
-      <c r="DV41" s="49"/>
-      <c r="DW41" s="49"/>
-      <c r="DX41" s="50"/>
+      <c r="DK41" s="60"/>
+      <c r="DL41" s="61"/>
+      <c r="DM41" s="61"/>
+      <c r="DN41" s="61"/>
+      <c r="DO41" s="61"/>
+      <c r="DP41" s="61"/>
+      <c r="DQ41" s="62"/>
+      <c r="DR41" s="60"/>
+      <c r="DS41" s="61"/>
+      <c r="DT41" s="61"/>
+      <c r="DU41" s="61"/>
+      <c r="DV41" s="61"/>
+      <c r="DW41" s="61"/>
+      <c r="DX41" s="62"/>
       <c r="DY41" s="2"/>
       <c r="DZ41" s="1"/>
       <c r="EA41" s="1"/>
@@ -8101,8 +8096,8 @@
       <c r="EL41" s="3"/>
     </row>
     <row r="42" spans="1:142" ht="15" thickBot="1">
-      <c r="A42" s="20"/>
-      <c r="B42" s="36" t="s">
+      <c r="A42" s="33"/>
+      <c r="B42" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C42" s="2"/>
@@ -8140,13 +8135,13 @@
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="3"/>
-      <c r="AL42" s="57"/>
-      <c r="AM42" s="58"/>
-      <c r="AN42" s="58"/>
-      <c r="AO42" s="58"/>
-      <c r="AP42" s="58"/>
-      <c r="AQ42" s="58"/>
-      <c r="AR42" s="59"/>
+      <c r="AL42" s="52"/>
+      <c r="AM42" s="53"/>
+      <c r="AN42" s="53"/>
+      <c r="AO42" s="53"/>
+      <c r="AP42" s="53"/>
+      <c r="AQ42" s="53"/>
+      <c r="AR42" s="54"/>
       <c r="AS42" s="2"/>
       <c r="AT42" s="1"/>
       <c r="AU42" s="1"/>
@@ -8217,20 +8212,20 @@
       <c r="DH42" s="1"/>
       <c r="DI42" s="1"/>
       <c r="DJ42" s="3"/>
-      <c r="DK42" s="48"/>
-      <c r="DL42" s="49"/>
-      <c r="DM42" s="49"/>
-      <c r="DN42" s="49"/>
-      <c r="DO42" s="49"/>
-      <c r="DP42" s="49"/>
-      <c r="DQ42" s="50"/>
-      <c r="DR42" s="48"/>
-      <c r="DS42" s="49"/>
-      <c r="DT42" s="49"/>
-      <c r="DU42" s="49"/>
-      <c r="DV42" s="49"/>
-      <c r="DW42" s="49"/>
-      <c r="DX42" s="50"/>
+      <c r="DK42" s="60"/>
+      <c r="DL42" s="61"/>
+      <c r="DM42" s="61"/>
+      <c r="DN42" s="61"/>
+      <c r="DO42" s="61"/>
+      <c r="DP42" s="61"/>
+      <c r="DQ42" s="62"/>
+      <c r="DR42" s="60"/>
+      <c r="DS42" s="61"/>
+      <c r="DT42" s="61"/>
+      <c r="DU42" s="61"/>
+      <c r="DV42" s="61"/>
+      <c r="DW42" s="61"/>
+      <c r="DX42" s="62"/>
       <c r="DY42" s="2"/>
       <c r="DZ42" s="1"/>
       <c r="EA42" s="1"/>
@@ -8247,10 +8242,10 @@
       <c r="EL42" s="3"/>
     </row>
     <row r="43" spans="1:142" ht="15" thickBot="1">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="2"/>
@@ -8288,13 +8283,13 @@
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="3"/>
-      <c r="AL43" s="57"/>
-      <c r="AM43" s="58"/>
-      <c r="AN43" s="58"/>
-      <c r="AO43" s="58"/>
-      <c r="AP43" s="58"/>
-      <c r="AQ43" s="58"/>
-      <c r="AR43" s="59"/>
+      <c r="AL43" s="52"/>
+      <c r="AM43" s="53"/>
+      <c r="AN43" s="53"/>
+      <c r="AO43" s="53"/>
+      <c r="AP43" s="53"/>
+      <c r="AQ43" s="53"/>
+      <c r="AR43" s="54"/>
       <c r="AS43" s="2"/>
       <c r="AT43" s="1"/>
       <c r="AU43" s="1"/>
@@ -8365,20 +8360,20 @@
       <c r="DH43" s="1"/>
       <c r="DI43" s="1"/>
       <c r="DJ43" s="3"/>
-      <c r="DK43" s="48"/>
-      <c r="DL43" s="49"/>
-      <c r="DM43" s="49"/>
-      <c r="DN43" s="49"/>
-      <c r="DO43" s="49"/>
-      <c r="DP43" s="49"/>
-      <c r="DQ43" s="50"/>
-      <c r="DR43" s="48"/>
-      <c r="DS43" s="49"/>
-      <c r="DT43" s="49"/>
-      <c r="DU43" s="49"/>
-      <c r="DV43" s="49"/>
-      <c r="DW43" s="49"/>
-      <c r="DX43" s="50"/>
+      <c r="DK43" s="60"/>
+      <c r="DL43" s="61"/>
+      <c r="DM43" s="61"/>
+      <c r="DN43" s="61"/>
+      <c r="DO43" s="61"/>
+      <c r="DP43" s="61"/>
+      <c r="DQ43" s="62"/>
+      <c r="DR43" s="60"/>
+      <c r="DS43" s="61"/>
+      <c r="DT43" s="61"/>
+      <c r="DU43" s="61"/>
+      <c r="DV43" s="61"/>
+      <c r="DW43" s="61"/>
+      <c r="DX43" s="62"/>
       <c r="DY43" s="2"/>
       <c r="DZ43" s="1"/>
       <c r="EA43" s="1"/>
@@ -8395,8 +8390,8 @@
       <c r="EL43" s="3"/>
     </row>
     <row r="44" spans="1:142" ht="15" thickBot="1">
-      <c r="A44" s="20"/>
-      <c r="B44" s="36" t="s">
+      <c r="A44" s="33"/>
+      <c r="B44" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C44" s="2"/>
@@ -8434,13 +8429,13 @@
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="3"/>
-      <c r="AL44" s="57"/>
-      <c r="AM44" s="58"/>
-      <c r="AN44" s="58"/>
-      <c r="AO44" s="58"/>
-      <c r="AP44" s="58"/>
-      <c r="AQ44" s="58"/>
-      <c r="AR44" s="59"/>
+      <c r="AL44" s="52"/>
+      <c r="AM44" s="53"/>
+      <c r="AN44" s="53"/>
+      <c r="AO44" s="53"/>
+      <c r="AP44" s="53"/>
+      <c r="AQ44" s="53"/>
+      <c r="AR44" s="54"/>
       <c r="AS44" s="2"/>
       <c r="AT44" s="1"/>
       <c r="AU44" s="1"/>
@@ -8511,20 +8506,20 @@
       <c r="DH44" s="1"/>
       <c r="DI44" s="1"/>
       <c r="DJ44" s="3"/>
-      <c r="DK44" s="48"/>
-      <c r="DL44" s="49"/>
-      <c r="DM44" s="49"/>
-      <c r="DN44" s="49"/>
-      <c r="DO44" s="49"/>
-      <c r="DP44" s="49"/>
-      <c r="DQ44" s="50"/>
-      <c r="DR44" s="48"/>
-      <c r="DS44" s="49"/>
-      <c r="DT44" s="49"/>
-      <c r="DU44" s="49"/>
-      <c r="DV44" s="49"/>
-      <c r="DW44" s="49"/>
-      <c r="DX44" s="50"/>
+      <c r="DK44" s="60"/>
+      <c r="DL44" s="61"/>
+      <c r="DM44" s="61"/>
+      <c r="DN44" s="61"/>
+      <c r="DO44" s="61"/>
+      <c r="DP44" s="61"/>
+      <c r="DQ44" s="62"/>
+      <c r="DR44" s="60"/>
+      <c r="DS44" s="61"/>
+      <c r="DT44" s="61"/>
+      <c r="DU44" s="61"/>
+      <c r="DV44" s="61"/>
+      <c r="DW44" s="61"/>
+      <c r="DX44" s="62"/>
       <c r="DY44" s="2"/>
       <c r="DZ44" s="1"/>
       <c r="EA44" s="1"/>
@@ -8541,8 +8536,8 @@
       <c r="EL44" s="3"/>
     </row>
     <row r="45" spans="1:142" ht="15" thickBot="1">
-      <c r="A45" s="38"/>
-      <c r="B45" s="37" t="s">
+      <c r="A45" s="34"/>
+      <c r="B45" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C45" s="2"/>
@@ -8580,13 +8575,13 @@
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="3"/>
-      <c r="AL45" s="57"/>
-      <c r="AM45" s="58"/>
-      <c r="AN45" s="58"/>
-      <c r="AO45" s="58"/>
-      <c r="AP45" s="58"/>
-      <c r="AQ45" s="58"/>
-      <c r="AR45" s="59"/>
+      <c r="AL45" s="52"/>
+      <c r="AM45" s="53"/>
+      <c r="AN45" s="53"/>
+      <c r="AO45" s="53"/>
+      <c r="AP45" s="53"/>
+      <c r="AQ45" s="53"/>
+      <c r="AR45" s="54"/>
       <c r="AS45" s="2"/>
       <c r="AT45" s="1"/>
       <c r="AU45" s="1"/>
@@ -8657,20 +8652,20 @@
       <c r="DH45" s="1"/>
       <c r="DI45" s="1"/>
       <c r="DJ45" s="3"/>
-      <c r="DK45" s="48"/>
-      <c r="DL45" s="49"/>
-      <c r="DM45" s="49"/>
-      <c r="DN45" s="49"/>
-      <c r="DO45" s="49"/>
-      <c r="DP45" s="49"/>
-      <c r="DQ45" s="50"/>
-      <c r="DR45" s="48"/>
-      <c r="DS45" s="49"/>
-      <c r="DT45" s="49"/>
-      <c r="DU45" s="49"/>
-      <c r="DV45" s="49"/>
-      <c r="DW45" s="49"/>
-      <c r="DX45" s="50"/>
+      <c r="DK45" s="60"/>
+      <c r="DL45" s="61"/>
+      <c r="DM45" s="61"/>
+      <c r="DN45" s="61"/>
+      <c r="DO45" s="61"/>
+      <c r="DP45" s="61"/>
+      <c r="DQ45" s="62"/>
+      <c r="DR45" s="60"/>
+      <c r="DS45" s="61"/>
+      <c r="DT45" s="61"/>
+      <c r="DU45" s="61"/>
+      <c r="DV45" s="61"/>
+      <c r="DW45" s="61"/>
+      <c r="DX45" s="62"/>
       <c r="DY45" s="2"/>
       <c r="DZ45" s="1"/>
       <c r="EA45" s="1"/>
@@ -8679,7 +8674,7 @@
       <c r="ED45" s="1"/>
       <c r="EE45" s="3"/>
       <c r="EF45" s="2"/>
-      <c r="EG45" s="34"/>
+      <c r="EG45" s="1"/>
       <c r="EH45" s="1"/>
       <c r="EI45" s="1"/>
       <c r="EJ45" s="1"/>
@@ -8687,8 +8682,8 @@
       <c r="EL45" s="3"/>
     </row>
     <row r="46" spans="1:142" ht="15" thickBot="1">
-      <c r="A46" s="39"/>
-      <c r="B46" s="36" t="s">
+      <c r="A46" s="35"/>
+      <c r="B46" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C46" s="4"/>
@@ -8726,13 +8721,13 @@
       <c r="AI46" s="5"/>
       <c r="AJ46" s="5"/>
       <c r="AK46" s="6"/>
-      <c r="AL46" s="60"/>
-      <c r="AM46" s="61"/>
-      <c r="AN46" s="61"/>
-      <c r="AO46" s="61"/>
-      <c r="AP46" s="61"/>
-      <c r="AQ46" s="61"/>
-      <c r="AR46" s="62"/>
+      <c r="AL46" s="55"/>
+      <c r="AM46" s="56"/>
+      <c r="AN46" s="56"/>
+      <c r="AO46" s="56"/>
+      <c r="AP46" s="56"/>
+      <c r="AQ46" s="56"/>
+      <c r="AR46" s="57"/>
       <c r="AS46" s="4"/>
       <c r="AT46" s="5"/>
       <c r="AU46" s="5"/>
@@ -8803,20 +8798,20 @@
       <c r="DH46" s="5"/>
       <c r="DI46" s="5"/>
       <c r="DJ46" s="6"/>
-      <c r="DK46" s="51"/>
-      <c r="DL46" s="52"/>
-      <c r="DM46" s="52"/>
-      <c r="DN46" s="52"/>
-      <c r="DO46" s="52"/>
-      <c r="DP46" s="52"/>
-      <c r="DQ46" s="53"/>
-      <c r="DR46" s="51"/>
-      <c r="DS46" s="52"/>
-      <c r="DT46" s="52"/>
-      <c r="DU46" s="52"/>
-      <c r="DV46" s="52"/>
-      <c r="DW46" s="52"/>
-      <c r="DX46" s="53"/>
+      <c r="DK46" s="63"/>
+      <c r="DL46" s="64"/>
+      <c r="DM46" s="64"/>
+      <c r="DN46" s="64"/>
+      <c r="DO46" s="64"/>
+      <c r="DP46" s="64"/>
+      <c r="DQ46" s="65"/>
+      <c r="DR46" s="63"/>
+      <c r="DS46" s="64"/>
+      <c r="DT46" s="64"/>
+      <c r="DU46" s="64"/>
+      <c r="DV46" s="64"/>
+      <c r="DW46" s="64"/>
+      <c r="DX46" s="65"/>
       <c r="DY46" s="4"/>
       <c r="DZ46" s="5"/>
       <c r="EA46" s="5"/>
@@ -8832,33 +8827,20 @@
       <c r="EK46" s="5"/>
       <c r="EL46" s="6"/>
     </row>
-    <row r="47" spans="1:142">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="31"/>
-      <c r="B49" s="31"/>
-    </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="BU3:CA3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="X3:AD3"/>
+    <mergeCell ref="AE3:AK3"/>
+    <mergeCell ref="AL3:AR3"/>
+    <mergeCell ref="AS3:AY3"/>
+    <mergeCell ref="AZ3:BF3"/>
+    <mergeCell ref="BG3:BM3"/>
+    <mergeCell ref="BN3:BT3"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="DR3:DX3"/>
     <mergeCell ref="DY3:EE3"/>
@@ -8875,18 +8857,23 @@
     <mergeCell ref="CW3:DC3"/>
     <mergeCell ref="DD3:DJ3"/>
     <mergeCell ref="DK3:DQ3"/>
-    <mergeCell ref="AL3:AR3"/>
-    <mergeCell ref="AS3:AY3"/>
-    <mergeCell ref="AZ3:BF3"/>
-    <mergeCell ref="BG3:BM3"/>
-    <mergeCell ref="BN3:BT3"/>
-    <mergeCell ref="BU3:CA3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="X3:AD3"/>
-    <mergeCell ref="AE3:AK3"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A43:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8906,81 +8893,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="67"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="71">
         <v>1</v>
       </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="71"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="67"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="72">
         <v>45524</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="72"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="73">
         <v>45671</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="73"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="67"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="68"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="9" t="s">
@@ -9019,7 +9006,7 @@
       <c r="A18" s="11">
         <v>3</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -9157,7 +9144,7 @@
       <c r="A30" s="11">
         <v>15</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="11" t="s">
         <v>85</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -9239,11 +9226,11 @@
       <c r="C38" s="11"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="9" t="s">

</xml_diff>

<commit_message>
Updatet Doku and Zeitplan and added Comments in Code
</commit_message>
<xml_diff>
--- a/documentation/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
+++ b/documentation/Marvin_AudioAnlage_Anforderungen_NoraHueppi_20240917.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd4b8c2adf92642a/Berufsschule/BuP/5_Semester/Marvin/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{222596FB-A639-49AC-A788-7FE2CF6654A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A3A450E-FBDB-493E-BB77-A482F3AE20F9}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{222596FB-A639-49AC-A788-7FE2CF6654A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9D91153-441C-47D1-B360-ED162A866621}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="4" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="100">
   <si>
     <t>Zeitplan</t>
   </si>
@@ -137,15 +137,9 @@
     <t>KW 3</t>
   </si>
   <si>
-    <t>Stückliste</t>
-  </si>
-  <si>
     <t>Schema</t>
   </si>
   <si>
-    <t>Layout</t>
-  </si>
-  <si>
     <t>Soll</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
   </si>
   <si>
     <t>Dokumentation</t>
-  </si>
-  <si>
-    <t>Audio aufnehmen</t>
   </si>
   <si>
     <t>Präsentation vorbereiten</t>
@@ -447,6 +438,21 @@
   </si>
   <si>
     <t>Es soll eine Zeitschalterfunktion geben, mit der die Anlage zu einer bestimmten Uhrzeit aktiviert wird.</t>
+  </si>
+  <si>
+    <t>BoM</t>
+  </si>
+  <si>
+    <t>Gelötet</t>
+  </si>
+  <si>
+    <t>Audio aufnehmen und bearbeiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 </t>
+  </si>
+  <si>
+    <t>awq</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1378,50 +1384,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1432,32 +1402,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1475,6 +1427,60 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1504,6 +1510,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2203,9 +2219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730C7784-EAA3-4F75-A441-9364A27E8BAB}">
   <dimension ref="A1:ES37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="95" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="CU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DB13" sqref="DB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -2336,10 +2352,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:149" ht="21">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="107"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -2627,200 +2643,200 @@
     </row>
     <row r="3" spans="1:149" ht="15" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B3" s="67">
         <f>SUM(C6:EL6,C8:EL8,C10:EL10,C12:EL12,C14:EL14,C16:EL16,C18:EL18,C20:EL20,C22:EL22,C24:EL24,C26:EL26,C28:EL28,C30:EL30,C32:EL32,C34:EL34,C36:EL36)</f>
-        <v>121</v>
-      </c>
-      <c r="C3" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="80" t="s">
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="77" t="s">
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="79"/>
-      <c r="X3" s="77" t="s">
+      <c r="R3" s="99"/>
+      <c r="S3" s="99"/>
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
-      <c r="AB3" s="78"/>
-      <c r="AC3" s="78"/>
-      <c r="AD3" s="79"/>
-      <c r="AE3" s="77" t="s">
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="99"/>
+      <c r="AA3" s="99"/>
+      <c r="AB3" s="99"/>
+      <c r="AC3" s="99"/>
+      <c r="AD3" s="100"/>
+      <c r="AE3" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="AF3" s="78"/>
-      <c r="AG3" s="78"/>
-      <c r="AH3" s="78"/>
-      <c r="AI3" s="78"/>
-      <c r="AJ3" s="78"/>
-      <c r="AK3" s="79"/>
-      <c r="AL3" s="77" t="s">
+      <c r="AF3" s="99"/>
+      <c r="AG3" s="99"/>
+      <c r="AH3" s="99"/>
+      <c r="AI3" s="99"/>
+      <c r="AJ3" s="99"/>
+      <c r="AK3" s="100"/>
+      <c r="AL3" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="AM3" s="78"/>
-      <c r="AN3" s="78"/>
-      <c r="AO3" s="78"/>
-      <c r="AP3" s="78"/>
-      <c r="AQ3" s="78"/>
-      <c r="AR3" s="79"/>
-      <c r="AS3" s="77" t="s">
+      <c r="AM3" s="99"/>
+      <c r="AN3" s="99"/>
+      <c r="AO3" s="99"/>
+      <c r="AP3" s="99"/>
+      <c r="AQ3" s="99"/>
+      <c r="AR3" s="100"/>
+      <c r="AS3" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="AT3" s="78"/>
-      <c r="AU3" s="78"/>
-      <c r="AV3" s="78"/>
-      <c r="AW3" s="78"/>
-      <c r="AX3" s="78"/>
-      <c r="AY3" s="79"/>
-      <c r="AZ3" s="77" t="s">
+      <c r="AT3" s="99"/>
+      <c r="AU3" s="99"/>
+      <c r="AV3" s="99"/>
+      <c r="AW3" s="99"/>
+      <c r="AX3" s="99"/>
+      <c r="AY3" s="100"/>
+      <c r="AZ3" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="BA3" s="78"/>
-      <c r="BB3" s="78"/>
-      <c r="BC3" s="78"/>
-      <c r="BD3" s="78"/>
-      <c r="BE3" s="78"/>
-      <c r="BF3" s="79"/>
-      <c r="BG3" s="77" t="s">
+      <c r="BA3" s="99"/>
+      <c r="BB3" s="99"/>
+      <c r="BC3" s="99"/>
+      <c r="BD3" s="99"/>
+      <c r="BE3" s="99"/>
+      <c r="BF3" s="100"/>
+      <c r="BG3" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="BH3" s="78"/>
-      <c r="BI3" s="78"/>
-      <c r="BJ3" s="78"/>
-      <c r="BK3" s="78"/>
-      <c r="BL3" s="78"/>
-      <c r="BM3" s="79"/>
-      <c r="BN3" s="77" t="s">
+      <c r="BH3" s="99"/>
+      <c r="BI3" s="99"/>
+      <c r="BJ3" s="99"/>
+      <c r="BK3" s="99"/>
+      <c r="BL3" s="99"/>
+      <c r="BM3" s="100"/>
+      <c r="BN3" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="BO3" s="78"/>
-      <c r="BP3" s="78"/>
-      <c r="BQ3" s="78"/>
-      <c r="BR3" s="78"/>
-      <c r="BS3" s="78"/>
-      <c r="BT3" s="79"/>
-      <c r="BU3" s="77" t="s">
+      <c r="BO3" s="99"/>
+      <c r="BP3" s="99"/>
+      <c r="BQ3" s="99"/>
+      <c r="BR3" s="99"/>
+      <c r="BS3" s="99"/>
+      <c r="BT3" s="100"/>
+      <c r="BU3" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="BV3" s="78"/>
-      <c r="BW3" s="78"/>
-      <c r="BX3" s="78"/>
-      <c r="BY3" s="78"/>
-      <c r="BZ3" s="78"/>
-      <c r="CA3" s="79"/>
-      <c r="CB3" s="77" t="s">
+      <c r="BV3" s="99"/>
+      <c r="BW3" s="99"/>
+      <c r="BX3" s="99"/>
+      <c r="BY3" s="99"/>
+      <c r="BZ3" s="99"/>
+      <c r="CA3" s="100"/>
+      <c r="CB3" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="CC3" s="78"/>
-      <c r="CD3" s="78"/>
-      <c r="CE3" s="78"/>
-      <c r="CF3" s="78"/>
-      <c r="CG3" s="78"/>
-      <c r="CH3" s="79"/>
-      <c r="CI3" s="77" t="s">
+      <c r="CC3" s="99"/>
+      <c r="CD3" s="99"/>
+      <c r="CE3" s="99"/>
+      <c r="CF3" s="99"/>
+      <c r="CG3" s="99"/>
+      <c r="CH3" s="100"/>
+      <c r="CI3" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="CJ3" s="78"/>
-      <c r="CK3" s="78"/>
-      <c r="CL3" s="78"/>
-      <c r="CM3" s="78"/>
-      <c r="CN3" s="78"/>
-      <c r="CO3" s="79"/>
-      <c r="CP3" s="77" t="s">
+      <c r="CJ3" s="99"/>
+      <c r="CK3" s="99"/>
+      <c r="CL3" s="99"/>
+      <c r="CM3" s="99"/>
+      <c r="CN3" s="99"/>
+      <c r="CO3" s="100"/>
+      <c r="CP3" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="CQ3" s="78"/>
-      <c r="CR3" s="78"/>
-      <c r="CS3" s="78"/>
-      <c r="CT3" s="78"/>
-      <c r="CU3" s="78"/>
-      <c r="CV3" s="79"/>
-      <c r="CW3" s="77" t="s">
+      <c r="CQ3" s="99"/>
+      <c r="CR3" s="99"/>
+      <c r="CS3" s="99"/>
+      <c r="CT3" s="99"/>
+      <c r="CU3" s="99"/>
+      <c r="CV3" s="100"/>
+      <c r="CW3" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="CX3" s="78"/>
-      <c r="CY3" s="78"/>
-      <c r="CZ3" s="78"/>
-      <c r="DA3" s="78"/>
-      <c r="DB3" s="78"/>
-      <c r="DC3" s="79"/>
-      <c r="DD3" s="77" t="s">
+      <c r="CX3" s="99"/>
+      <c r="CY3" s="99"/>
+      <c r="CZ3" s="99"/>
+      <c r="DA3" s="99"/>
+      <c r="DB3" s="99"/>
+      <c r="DC3" s="100"/>
+      <c r="DD3" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="DE3" s="78"/>
-      <c r="DF3" s="78"/>
-      <c r="DG3" s="78"/>
-      <c r="DH3" s="78"/>
-      <c r="DI3" s="78"/>
-      <c r="DJ3" s="79"/>
-      <c r="DK3" s="77" t="s">
+      <c r="DE3" s="99"/>
+      <c r="DF3" s="99"/>
+      <c r="DG3" s="99"/>
+      <c r="DH3" s="99"/>
+      <c r="DI3" s="99"/>
+      <c r="DJ3" s="100"/>
+      <c r="DK3" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="DL3" s="78"/>
-      <c r="DM3" s="78"/>
-      <c r="DN3" s="78"/>
-      <c r="DO3" s="78"/>
-      <c r="DP3" s="78"/>
-      <c r="DQ3" s="79"/>
-      <c r="DR3" s="77" t="s">
+      <c r="DL3" s="99"/>
+      <c r="DM3" s="99"/>
+      <c r="DN3" s="99"/>
+      <c r="DO3" s="99"/>
+      <c r="DP3" s="99"/>
+      <c r="DQ3" s="100"/>
+      <c r="DR3" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="DS3" s="78"/>
-      <c r="DT3" s="78"/>
-      <c r="DU3" s="78"/>
-      <c r="DV3" s="78"/>
-      <c r="DW3" s="78"/>
-      <c r="DX3" s="79"/>
-      <c r="DY3" s="81" t="s">
+      <c r="DS3" s="99"/>
+      <c r="DT3" s="99"/>
+      <c r="DU3" s="99"/>
+      <c r="DV3" s="99"/>
+      <c r="DW3" s="99"/>
+      <c r="DX3" s="100"/>
+      <c r="DY3" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="DZ3" s="82"/>
-      <c r="EA3" s="82"/>
-      <c r="EB3" s="82"/>
-      <c r="EC3" s="82"/>
-      <c r="ED3" s="82"/>
-      <c r="EE3" s="83"/>
-      <c r="EF3" s="81" t="s">
+      <c r="DZ3" s="102"/>
+      <c r="EA3" s="102"/>
+      <c r="EB3" s="102"/>
+      <c r="EC3" s="102"/>
+      <c r="ED3" s="102"/>
+      <c r="EE3" s="103"/>
+      <c r="EF3" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="EG3" s="82"/>
-      <c r="EH3" s="82"/>
-      <c r="EI3" s="82"/>
-      <c r="EJ3" s="82"/>
-      <c r="EK3" s="82"/>
-      <c r="EL3" s="83"/>
+      <c r="EG3" s="102"/>
+      <c r="EH3" s="102"/>
+      <c r="EI3" s="102"/>
+      <c r="EJ3" s="102"/>
+      <c r="EK3" s="102"/>
+      <c r="EL3" s="103"/>
     </row>
     <row r="4" spans="1:149" ht="15" thickBot="1">
       <c r="A4" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B4" s="64">
         <f>SUM(C7:EL7,C9:EL9,C11:EL11,C13:EL13,C15:EL15,C17:EL17,C19:EL19,C21:EL21,C23:EL23,C25:EL25,C27:EL27,C29:EL29,C31:EL31,C33:EL33,C35:EL35,C37:EL37)</f>
-        <v>33</v>
+        <v>148</v>
       </c>
       <c r="C4" s="35" t="s">
         <v>1</v>
@@ -3244,156 +3260,156 @@
       </c>
     </row>
     <row r="5" spans="1:149" ht="19" thickBot="1">
-      <c r="A5" s="94" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="93"/>
-      <c r="X5" s="91"/>
-      <c r="Y5" s="92"/>
-      <c r="Z5" s="92"/>
-      <c r="AA5" s="92"/>
-      <c r="AB5" s="92"/>
-      <c r="AC5" s="92"/>
-      <c r="AD5" s="93"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="92"/>
-      <c r="AG5" s="92"/>
-      <c r="AH5" s="92"/>
-      <c r="AI5" s="92"/>
-      <c r="AJ5" s="92"/>
-      <c r="AK5" s="93"/>
-      <c r="AL5" s="103" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM5" s="104"/>
-      <c r="AN5" s="104"/>
-      <c r="AO5" s="104"/>
-      <c r="AP5" s="104"/>
-      <c r="AQ5" s="104"/>
-      <c r="AR5" s="105"/>
-      <c r="AS5" s="91"/>
-      <c r="AT5" s="92"/>
-      <c r="AU5" s="92"/>
-      <c r="AV5" s="92"/>
-      <c r="AW5" s="92"/>
-      <c r="AX5" s="92"/>
-      <c r="AY5" s="93"/>
-      <c r="AZ5" s="91"/>
-      <c r="BA5" s="92"/>
-      <c r="BB5" s="92"/>
-      <c r="BC5" s="92"/>
-      <c r="BD5" s="92"/>
-      <c r="BE5" s="92"/>
-      <c r="BF5" s="93"/>
-      <c r="BG5" s="91"/>
-      <c r="BH5" s="92"/>
-      <c r="BI5" s="92"/>
-      <c r="BJ5" s="92"/>
-      <c r="BK5" s="92"/>
-      <c r="BL5" s="92"/>
-      <c r="BM5" s="93"/>
-      <c r="BN5" s="91"/>
-      <c r="BO5" s="92"/>
-      <c r="BP5" s="92"/>
-      <c r="BQ5" s="92"/>
-      <c r="BR5" s="92"/>
-      <c r="BS5" s="92"/>
-      <c r="BT5" s="93"/>
-      <c r="BU5" s="91"/>
-      <c r="BV5" s="92"/>
-      <c r="BW5" s="92"/>
-      <c r="BX5" s="92"/>
-      <c r="BY5" s="92"/>
-      <c r="BZ5" s="92"/>
-      <c r="CA5" s="93"/>
-      <c r="CB5" s="91"/>
-      <c r="CC5" s="92"/>
-      <c r="CD5" s="92"/>
-      <c r="CE5" s="92"/>
-      <c r="CF5" s="92"/>
-      <c r="CG5" s="92"/>
-      <c r="CH5" s="93"/>
-      <c r="CI5" s="91"/>
-      <c r="CJ5" s="92"/>
-      <c r="CK5" s="92"/>
-      <c r="CL5" s="92"/>
-      <c r="CM5" s="92"/>
-      <c r="CN5" s="92"/>
-      <c r="CO5" s="93"/>
-      <c r="CP5" s="91"/>
-      <c r="CQ5" s="92"/>
-      <c r="CR5" s="92"/>
-      <c r="CS5" s="92"/>
-      <c r="CT5" s="92"/>
-      <c r="CU5" s="92"/>
-      <c r="CV5" s="93"/>
-      <c r="CW5" s="91"/>
-      <c r="CX5" s="92"/>
-      <c r="CY5" s="92"/>
-      <c r="CZ5" s="92"/>
-      <c r="DA5" s="92"/>
-      <c r="DB5" s="92"/>
-      <c r="DC5" s="93"/>
-      <c r="DD5" s="91"/>
-      <c r="DE5" s="92"/>
-      <c r="DF5" s="92"/>
-      <c r="DG5" s="92"/>
-      <c r="DH5" s="92"/>
-      <c r="DI5" s="92"/>
-      <c r="DJ5" s="93"/>
-      <c r="DK5" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="DL5" s="89"/>
-      <c r="DM5" s="89"/>
-      <c r="DN5" s="89"/>
-      <c r="DO5" s="89"/>
-      <c r="DP5" s="89"/>
-      <c r="DQ5" s="90"/>
-      <c r="DR5" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="DS5" s="89"/>
-      <c r="DT5" s="89"/>
-      <c r="DU5" s="89"/>
-      <c r="DV5" s="89"/>
-      <c r="DW5" s="89"/>
-      <c r="DX5" s="90"/>
-      <c r="DY5" s="91"/>
-      <c r="DZ5" s="92"/>
-      <c r="EA5" s="92"/>
-      <c r="EB5" s="92"/>
-      <c r="EC5" s="92"/>
-      <c r="ED5" s="92"/>
-      <c r="EE5" s="93"/>
-      <c r="EF5" s="91"/>
-      <c r="EG5" s="92"/>
-      <c r="EH5" s="92"/>
-      <c r="EI5" s="92"/>
-      <c r="EJ5" s="92"/>
-      <c r="EK5" s="92"/>
-      <c r="EL5" s="93"/>
+      <c r="A5" s="105" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="106"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="80"/>
+      <c r="Z5" s="80"/>
+      <c r="AA5" s="80"/>
+      <c r="AB5" s="80"/>
+      <c r="AC5" s="80"/>
+      <c r="AD5" s="81"/>
+      <c r="AE5" s="79"/>
+      <c r="AF5" s="80"/>
+      <c r="AG5" s="80"/>
+      <c r="AH5" s="80"/>
+      <c r="AI5" s="80"/>
+      <c r="AJ5" s="80"/>
+      <c r="AK5" s="81"/>
+      <c r="AL5" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="86"/>
+      <c r="AO5" s="86"/>
+      <c r="AP5" s="86"/>
+      <c r="AQ5" s="86"/>
+      <c r="AR5" s="87"/>
+      <c r="AS5" s="79"/>
+      <c r="AT5" s="80"/>
+      <c r="AU5" s="80"/>
+      <c r="AV5" s="80"/>
+      <c r="AW5" s="80"/>
+      <c r="AX5" s="80"/>
+      <c r="AY5" s="81"/>
+      <c r="AZ5" s="79"/>
+      <c r="BA5" s="80"/>
+      <c r="BB5" s="80"/>
+      <c r="BC5" s="80"/>
+      <c r="BD5" s="80"/>
+      <c r="BE5" s="80"/>
+      <c r="BF5" s="81"/>
+      <c r="BG5" s="79"/>
+      <c r="BH5" s="80"/>
+      <c r="BI5" s="80"/>
+      <c r="BJ5" s="80"/>
+      <c r="BK5" s="80"/>
+      <c r="BL5" s="80"/>
+      <c r="BM5" s="81"/>
+      <c r="BN5" s="79"/>
+      <c r="BO5" s="80"/>
+      <c r="BP5" s="80"/>
+      <c r="BQ5" s="80"/>
+      <c r="BR5" s="80"/>
+      <c r="BS5" s="80"/>
+      <c r="BT5" s="81"/>
+      <c r="BU5" s="79"/>
+      <c r="BV5" s="80"/>
+      <c r="BW5" s="80"/>
+      <c r="BX5" s="80"/>
+      <c r="BY5" s="80"/>
+      <c r="BZ5" s="80"/>
+      <c r="CA5" s="81"/>
+      <c r="CB5" s="79"/>
+      <c r="CC5" s="80"/>
+      <c r="CD5" s="80"/>
+      <c r="CE5" s="80"/>
+      <c r="CF5" s="80"/>
+      <c r="CG5" s="80"/>
+      <c r="CH5" s="81"/>
+      <c r="CI5" s="79"/>
+      <c r="CJ5" s="80"/>
+      <c r="CK5" s="80"/>
+      <c r="CL5" s="80"/>
+      <c r="CM5" s="80"/>
+      <c r="CN5" s="80"/>
+      <c r="CO5" s="81"/>
+      <c r="CP5" s="79"/>
+      <c r="CQ5" s="80"/>
+      <c r="CR5" s="80"/>
+      <c r="CS5" s="80"/>
+      <c r="CT5" s="80"/>
+      <c r="CU5" s="80"/>
+      <c r="CV5" s="81"/>
+      <c r="CW5" s="79"/>
+      <c r="CX5" s="80"/>
+      <c r="CY5" s="80"/>
+      <c r="CZ5" s="80"/>
+      <c r="DA5" s="80"/>
+      <c r="DB5" s="80"/>
+      <c r="DC5" s="81"/>
+      <c r="DD5" s="79"/>
+      <c r="DE5" s="80"/>
+      <c r="DF5" s="80"/>
+      <c r="DG5" s="80"/>
+      <c r="DH5" s="80"/>
+      <c r="DI5" s="80"/>
+      <c r="DJ5" s="81"/>
+      <c r="DK5" s="82" t="s">
+        <v>90</v>
+      </c>
+      <c r="DL5" s="83"/>
+      <c r="DM5" s="83"/>
+      <c r="DN5" s="83"/>
+      <c r="DO5" s="83"/>
+      <c r="DP5" s="83"/>
+      <c r="DQ5" s="84"/>
+      <c r="DR5" s="82" t="s">
+        <v>90</v>
+      </c>
+      <c r="DS5" s="83"/>
+      <c r="DT5" s="83"/>
+      <c r="DU5" s="83"/>
+      <c r="DV5" s="83"/>
+      <c r="DW5" s="83"/>
+      <c r="DX5" s="84"/>
+      <c r="DY5" s="79"/>
+      <c r="DZ5" s="80"/>
+      <c r="EA5" s="80"/>
+      <c r="EB5" s="80"/>
+      <c r="EC5" s="80"/>
+      <c r="ED5" s="80"/>
+      <c r="EE5" s="81"/>
+      <c r="EF5" s="79"/>
+      <c r="EG5" s="80"/>
+      <c r="EH5" s="80"/>
+      <c r="EI5" s="80"/>
+      <c r="EJ5" s="80"/>
+      <c r="EK5" s="80"/>
+      <c r="EL5" s="81"/>
       <c r="EM5" s="2"/>
       <c r="EN5" s="2"/>
       <c r="EO5" s="2"/>
@@ -3403,11 +3419,11 @@
       <c r="ES5" s="2"/>
     </row>
     <row r="6" spans="1:149" ht="15" customHeight="1" thickBot="1">
-      <c r="A6" s="84" t="s">
-        <v>33</v>
+      <c r="A6" s="104" t="s">
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="71"/>
       <c r="D6" s="72"/>
@@ -3567,16 +3583,10 @@
       <c r="DZ6" s="17">
         <v>1</v>
       </c>
-      <c r="EA6" s="17">
-        <v>1</v>
-      </c>
-      <c r="EB6" s="17">
-        <v>1</v>
-      </c>
-      <c r="EC6" s="17">
-        <v>1</v>
-      </c>
-      <c r="ED6" s="15"/>
+      <c r="EA6" s="119"/>
+      <c r="EB6" s="119"/>
+      <c r="EC6" s="119"/>
+      <c r="ED6" s="119"/>
       <c r="EE6" s="16"/>
       <c r="EF6" s="14"/>
       <c r="EG6" s="15"/>
@@ -3587,9 +3597,9 @@
       <c r="EL6" s="16"/>
     </row>
     <row r="7" spans="1:149" ht="15" thickBot="1">
-      <c r="A7" s="85"/>
+      <c r="A7" s="92"/>
       <c r="B7" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
@@ -3640,49 +3650,63 @@
       <c r="AQ7" s="8"/>
       <c r="AR7" s="9"/>
       <c r="AS7" s="25"/>
-      <c r="AT7" s="21"/>
+      <c r="AT7" s="23">
+        <v>1</v>
+      </c>
       <c r="AU7" s="21"/>
       <c r="AV7" s="21"/>
       <c r="AW7" s="21"/>
       <c r="AX7" s="21"/>
       <c r="AY7" s="22"/>
       <c r="AZ7" s="20"/>
-      <c r="BA7" s="21"/>
+      <c r="BA7" s="23">
+        <v>1</v>
+      </c>
       <c r="BB7" s="21"/>
       <c r="BC7" s="21"/>
       <c r="BD7" s="21"/>
       <c r="BE7" s="21"/>
       <c r="BF7" s="22"/>
       <c r="BG7" s="20"/>
-      <c r="BH7" s="21"/>
+      <c r="BH7" s="23">
+        <v>1</v>
+      </c>
       <c r="BI7" s="21"/>
       <c r="BJ7" s="21"/>
       <c r="BK7" s="21"/>
       <c r="BL7" s="21"/>
       <c r="BM7" s="22"/>
       <c r="BN7" s="20"/>
-      <c r="BO7" s="21"/>
+      <c r="BO7" s="23">
+        <v>1</v>
+      </c>
       <c r="BP7" s="21"/>
       <c r="BQ7" s="21"/>
       <c r="BR7" s="21"/>
       <c r="BS7" s="21"/>
       <c r="BT7" s="22"/>
       <c r="BU7" s="20"/>
-      <c r="BV7" s="21"/>
+      <c r="BV7" s="23">
+        <v>1</v>
+      </c>
       <c r="BW7" s="21"/>
       <c r="BX7" s="21"/>
       <c r="BY7" s="21"/>
       <c r="BZ7" s="21"/>
       <c r="CA7" s="22"/>
       <c r="CB7" s="20"/>
-      <c r="CC7" s="21"/>
+      <c r="CC7" s="23">
+        <v>1</v>
+      </c>
       <c r="CD7" s="21"/>
       <c r="CE7" s="21"/>
       <c r="CF7" s="21"/>
       <c r="CG7" s="21"/>
       <c r="CH7" s="22"/>
       <c r="CI7" s="20"/>
-      <c r="CJ7" s="21"/>
+      <c r="CJ7" s="23">
+        <v>1</v>
+      </c>
       <c r="CK7" s="21"/>
       <c r="CL7" s="21"/>
       <c r="CM7" s="21"/>
@@ -3696,7 +3720,7 @@
       <c r="CU7" s="21"/>
       <c r="CV7" s="22"/>
       <c r="CW7" s="20"/>
-      <c r="CX7" s="21"/>
+      <c r="CX7" s="118"/>
       <c r="CY7" s="21"/>
       <c r="CZ7" s="21"/>
       <c r="DA7" s="21"/>
@@ -3712,19 +3736,33 @@
       <c r="DK7" s="7"/>
       <c r="DL7" s="8"/>
       <c r="DM7" s="8"/>
-      <c r="DN7" s="8"/>
-      <c r="DO7" s="8"/>
+      <c r="DN7" s="121">
+        <v>2</v>
+      </c>
+      <c r="DO7" s="121">
+        <v>2</v>
+      </c>
       <c r="DP7" s="8"/>
       <c r="DQ7" s="9"/>
       <c r="DR7" s="7"/>
       <c r="DS7" s="8"/>
       <c r="DT7" s="8"/>
       <c r="DU7" s="8"/>
-      <c r="DV7" s="8"/>
-      <c r="DW7" s="8"/>
-      <c r="DX7" s="9"/>
-      <c r="DY7" s="25"/>
-      <c r="DZ7" s="21"/>
+      <c r="DV7" s="121">
+        <v>2</v>
+      </c>
+      <c r="DW7" s="121">
+        <v>3</v>
+      </c>
+      <c r="DX7" s="122">
+        <v>5</v>
+      </c>
+      <c r="DY7" s="123">
+        <v>3</v>
+      </c>
+      <c r="DZ7" s="23">
+        <v>4</v>
+      </c>
       <c r="EA7" s="21"/>
       <c r="EB7" s="21"/>
       <c r="EC7" s="21"/>
@@ -3739,11 +3777,11 @@
       <c r="EL7" s="22"/>
     </row>
     <row r="8" spans="1:149" ht="15" thickBot="1">
-      <c r="A8" s="86" t="s">
-        <v>92</v>
+      <c r="A8" s="93" t="s">
+        <v>89</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="26">
@@ -3895,9 +3933,9 @@
       <c r="EL8" s="22"/>
     </row>
     <row r="9" spans="1:149" ht="15" thickBot="1">
-      <c r="A9" s="87"/>
+      <c r="A9" s="94"/>
       <c r="B9" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="23">
@@ -4051,11 +4089,11 @@
       <c r="EL9" s="22"/>
     </row>
     <row r="10" spans="1:149" ht="15" thickBot="1">
-      <c r="A10" s="96" t="s">
-        <v>36</v>
+      <c r="A10" s="91" t="s">
+        <v>33</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21"/>
@@ -4205,9 +4243,9 @@
       <c r="EL10" s="22"/>
     </row>
     <row r="11" spans="1:149" ht="15" thickBot="1">
-      <c r="A11" s="85"/>
+      <c r="A11" s="92"/>
       <c r="B11" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21"/>
@@ -4357,11 +4395,11 @@
       <c r="EL11" s="22"/>
     </row>
     <row r="12" spans="1:149" ht="15" thickBot="1">
-      <c r="A12" s="96" t="s">
-        <v>78</v>
+      <c r="A12" s="91" t="s">
+        <v>75</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
@@ -4511,9 +4549,9 @@
       <c r="EL12" s="22"/>
     </row>
     <row r="13" spans="1:149" ht="15" thickBot="1">
-      <c r="A13" s="85"/>
+      <c r="A13" s="92"/>
       <c r="B13" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="21"/>
@@ -4553,7 +4591,9 @@
       <c r="AF13" s="21"/>
       <c r="AG13" s="21"/>
       <c r="AH13" s="21"/>
-      <c r="AI13" s="21"/>
+      <c r="AI13" s="23">
+        <v>1</v>
+      </c>
       <c r="AJ13" s="21"/>
       <c r="AK13" s="24"/>
       <c r="AL13" s="7"/>
@@ -4624,7 +4664,9 @@
       <c r="CY13" s="21"/>
       <c r="CZ13" s="21"/>
       <c r="DA13" s="21"/>
-      <c r="DB13" s="21"/>
+      <c r="DB13" s="21" t="s">
+        <v>99</v>
+      </c>
       <c r="DC13" s="22"/>
       <c r="DD13" s="20"/>
       <c r="DE13" s="21"/>
@@ -4663,11 +4705,11 @@
       <c r="EL13" s="22"/>
     </row>
     <row r="14" spans="1:149" ht="15" thickBot="1">
-      <c r="A14" s="86" t="s">
-        <v>91</v>
+      <c r="A14" s="93" t="s">
+        <v>88</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
@@ -4817,9 +4859,9 @@
       <c r="EL14" s="22"/>
     </row>
     <row r="15" spans="1:149" ht="15" thickBot="1">
-      <c r="A15" s="87"/>
+      <c r="A15" s="94"/>
       <c r="B15" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
@@ -4967,11 +5009,11 @@
       <c r="EL15" s="22"/>
     </row>
     <row r="16" spans="1:149" ht="15" thickBot="1">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="65" t="s">
         <v>29</v>
-      </c>
-      <c r="B16" s="65" t="s">
-        <v>31</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21"/>
@@ -5123,7 +5165,7 @@
     <row r="17" spans="1:142" ht="15" thickBot="1">
       <c r="A17" s="97"/>
       <c r="B17" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21"/>
@@ -5171,7 +5213,9 @@
       <c r="AT17" s="21"/>
       <c r="AU17" s="21"/>
       <c r="AV17" s="21"/>
-      <c r="AW17" s="21"/>
+      <c r="AW17" s="23">
+        <v>4</v>
+      </c>
       <c r="AX17" s="21"/>
       <c r="AY17" s="22"/>
       <c r="AZ17" s="20"/>
@@ -5267,11 +5311,11 @@
       <c r="EL17" s="22"/>
     </row>
     <row r="18" spans="1:142" ht="15" thickBot="1">
-      <c r="A18" s="96" t="s">
-        <v>28</v>
+      <c r="A18" s="91" t="s">
+        <v>95</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
@@ -5319,15 +5363,13 @@
       <c r="AT18" s="21"/>
       <c r="AU18" s="21"/>
       <c r="AV18" s="21"/>
-      <c r="AW18" s="26">
-        <v>1</v>
-      </c>
+      <c r="AW18" s="118"/>
       <c r="AX18" s="21"/>
       <c r="AY18" s="22"/>
       <c r="AZ18" s="20"/>
       <c r="BA18" s="21"/>
       <c r="BB18" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BC18" s="63"/>
       <c r="BD18" s="21"/>
@@ -5421,7 +5463,7 @@
     <row r="19" spans="1:142" ht="15" thickBot="1">
       <c r="A19" s="97"/>
       <c r="B19" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
@@ -5565,11 +5607,11 @@
       <c r="EL19" s="22"/>
     </row>
     <row r="20" spans="1:142" ht="15" thickBot="1">
-      <c r="A20" s="96" t="s">
-        <v>30</v>
+      <c r="A20" s="91" t="s">
+        <v>96</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
@@ -5721,7 +5763,7 @@
     <row r="21" spans="1:142" ht="15" thickBot="1">
       <c r="A21" s="97"/>
       <c r="B21" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
@@ -5865,11 +5907,11 @@
       <c r="EL21" s="22"/>
     </row>
     <row r="22" spans="1:142" ht="15" thickBot="1">
-      <c r="A22" s="86" t="s">
-        <v>86</v>
+      <c r="A22" s="93" t="s">
+        <v>83</v>
       </c>
       <c r="B22" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
@@ -6019,9 +6061,9 @@
       <c r="EL22" s="22"/>
     </row>
     <row r="23" spans="1:142" ht="15" thickBot="1">
-      <c r="A23" s="87"/>
+      <c r="A23" s="94"/>
       <c r="B23" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
@@ -6081,14 +6123,22 @@
       <c r="BF23" s="22"/>
       <c r="BG23" s="20"/>
       <c r="BH23" s="21"/>
-      <c r="BI23" s="21"/>
-      <c r="BJ23" s="21"/>
-      <c r="BK23" s="21"/>
+      <c r="BI23" s="23">
+        <v>2</v>
+      </c>
+      <c r="BJ23" s="23">
+        <v>4</v>
+      </c>
+      <c r="BK23" s="23">
+        <v>4</v>
+      </c>
       <c r="BL23" s="21"/>
       <c r="BM23" s="22"/>
       <c r="BN23" s="20"/>
       <c r="BO23" s="21"/>
-      <c r="BP23" s="21"/>
+      <c r="BP23" s="23">
+        <v>1</v>
+      </c>
       <c r="BQ23" s="21"/>
       <c r="BR23" s="21"/>
       <c r="BS23" s="21"/>
@@ -6165,11 +6215,11 @@
       <c r="EL23" s="22"/>
     </row>
     <row r="24" spans="1:142" ht="15" thickBot="1">
-      <c r="A24" s="100" t="s">
-        <v>87</v>
+      <c r="A24" s="76" t="s">
+        <v>84</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
@@ -6232,9 +6282,11 @@
       <c r="BI24" s="21"/>
       <c r="BJ24" s="21"/>
       <c r="BK24" s="26">
-        <v>4</v>
-      </c>
-      <c r="BL24" s="21"/>
+        <v>10</v>
+      </c>
+      <c r="BL24" s="26">
+        <v>7</v>
+      </c>
       <c r="BM24" s="22"/>
       <c r="BN24" s="20"/>
       <c r="BO24" s="21"/>
@@ -6315,9 +6367,9 @@
       <c r="EL24" s="22"/>
     </row>
     <row r="25" spans="1:142" ht="15" thickBot="1">
-      <c r="A25" s="101"/>
+      <c r="A25" s="77"/>
       <c r="B25" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="21"/>
@@ -6379,13 +6431,21 @@
       <c r="BH25" s="21"/>
       <c r="BI25" s="21"/>
       <c r="BJ25" s="21"/>
-      <c r="BK25" s="21"/>
-      <c r="BL25" s="21"/>
+      <c r="BK25" s="23">
+        <v>10</v>
+      </c>
+      <c r="BL25" s="23">
+        <v>7</v>
+      </c>
       <c r="BM25" s="22"/>
       <c r="BN25" s="20"/>
       <c r="BO25" s="21"/>
-      <c r="BP25" s="21"/>
-      <c r="BQ25" s="21"/>
+      <c r="BP25" s="23">
+        <v>12</v>
+      </c>
+      <c r="BQ25" s="23">
+        <v>5</v>
+      </c>
       <c r="BR25" s="21"/>
       <c r="BS25" s="21"/>
       <c r="BT25" s="22"/>
@@ -6461,11 +6521,11 @@
       <c r="EL25" s="22"/>
     </row>
     <row r="26" spans="1:142" ht="15" thickBot="1">
-      <c r="A26" s="100" t="s">
-        <v>96</v>
+      <c r="A26" s="76" t="s">
+        <v>93</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
@@ -6615,9 +6675,9 @@
       <c r="EL26" s="22"/>
     </row>
     <row r="27" spans="1:142" ht="15" thickBot="1">
-      <c r="A27" s="102"/>
+      <c r="A27" s="78"/>
       <c r="B27" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
@@ -6685,10 +6745,18 @@
       <c r="BN27" s="20"/>
       <c r="BO27" s="21"/>
       <c r="BP27" s="21"/>
-      <c r="BQ27" s="21"/>
-      <c r="BR27" s="21"/>
-      <c r="BS27" s="21"/>
-      <c r="BT27" s="22"/>
+      <c r="BQ27" s="23">
+        <v>1</v>
+      </c>
+      <c r="BR27" s="23">
+        <v>2</v>
+      </c>
+      <c r="BS27" s="23">
+        <v>2</v>
+      </c>
+      <c r="BT27" s="120">
+        <v>4</v>
+      </c>
       <c r="BU27" s="20"/>
       <c r="BV27" s="21"/>
       <c r="BW27" s="21"/>
@@ -6761,11 +6829,11 @@
       <c r="EL27" s="22"/>
     </row>
     <row r="28" spans="1:142" ht="15" thickBot="1">
-      <c r="A28" s="86" t="s">
-        <v>34</v>
+      <c r="A28" s="93" t="s">
+        <v>97</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
@@ -6913,9 +6981,9 @@
       <c r="EL28" s="22"/>
     </row>
     <row r="29" spans="1:142" ht="15" thickBot="1">
-      <c r="A29" s="87"/>
+      <c r="A29" s="94"/>
       <c r="B29" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
@@ -6989,9 +7057,15 @@
       <c r="BT29" s="22"/>
       <c r="BU29" s="20"/>
       <c r="BV29" s="21"/>
-      <c r="BW29" s="21"/>
-      <c r="BX29" s="21"/>
-      <c r="BY29" s="21"/>
+      <c r="BW29" s="23">
+        <v>2</v>
+      </c>
+      <c r="BX29" s="23">
+        <v>3</v>
+      </c>
+      <c r="BY29" s="23">
+        <v>3</v>
+      </c>
       <c r="BZ29" s="21"/>
       <c r="CA29" s="22"/>
       <c r="CB29" s="20"/>
@@ -7059,11 +7133,11 @@
       <c r="EL29" s="22"/>
     </row>
     <row r="30" spans="1:142" ht="15" thickBot="1">
-      <c r="A30" s="86" t="s">
-        <v>88</v>
+      <c r="A30" s="93" t="s">
+        <v>85</v>
       </c>
       <c r="B30" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="21"/>
@@ -7233,9 +7307,9 @@
       <c r="EL30" s="22"/>
     </row>
     <row r="31" spans="1:142" ht="15" thickBot="1">
-      <c r="A31" s="87"/>
+      <c r="A31" s="94"/>
       <c r="B31" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="21"/>
@@ -7317,28 +7391,46 @@
       <c r="CB31" s="20"/>
       <c r="CC31" s="21"/>
       <c r="CD31" s="21"/>
-      <c r="CE31" s="21"/>
-      <c r="CF31" s="21"/>
+      <c r="CE31" s="23">
+        <v>2</v>
+      </c>
+      <c r="CF31" s="23">
+        <v>2</v>
+      </c>
       <c r="CG31" s="21"/>
       <c r="CH31" s="22"/>
-      <c r="CI31" s="20"/>
+      <c r="CI31" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="CJ31" s="21"/>
-      <c r="CK31" s="21"/>
-      <c r="CL31" s="21"/>
+      <c r="CK31" s="23">
+        <v>2</v>
+      </c>
+      <c r="CL31" s="23">
+        <v>2</v>
+      </c>
       <c r="CM31" s="21"/>
       <c r="CN31" s="21"/>
       <c r="CO31" s="22"/>
       <c r="CP31" s="20"/>
       <c r="CQ31" s="21"/>
-      <c r="CR31" s="21"/>
-      <c r="CS31" s="21"/>
+      <c r="CR31" s="23">
+        <v>2</v>
+      </c>
+      <c r="CS31" s="23">
+        <v>2</v>
+      </c>
       <c r="CT31" s="21"/>
       <c r="CU31" s="21"/>
       <c r="CV31" s="22"/>
       <c r="CW31" s="20"/>
       <c r="CX31" s="21"/>
-      <c r="CY31" s="21"/>
-      <c r="CZ31" s="21"/>
+      <c r="CY31" s="23">
+        <v>2</v>
+      </c>
+      <c r="CZ31" s="23">
+        <v>4</v>
+      </c>
       <c r="DA31" s="21"/>
       <c r="DB31" s="21"/>
       <c r="DC31" s="22"/>
@@ -7379,11 +7471,11 @@
       <c r="EL31" s="22"/>
     </row>
     <row r="32" spans="1:142" ht="15" thickBot="1">
-      <c r="A32" s="86" t="s">
-        <v>89</v>
+      <c r="A32" s="93" t="s">
+        <v>86</v>
       </c>
       <c r="B32" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="21"/>
@@ -7533,9 +7625,9 @@
       <c r="EL32" s="22"/>
     </row>
     <row r="33" spans="1:142" ht="15" thickBot="1">
-      <c r="A33" s="98"/>
+      <c r="A33" s="95"/>
       <c r="B33" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
@@ -7645,8 +7737,12 @@
       <c r="DD33" s="20"/>
       <c r="DE33" s="21"/>
       <c r="DF33" s="21"/>
-      <c r="DG33" s="21"/>
-      <c r="DH33" s="21"/>
+      <c r="DG33" s="23">
+        <v>1</v>
+      </c>
+      <c r="DH33" s="23">
+        <v>1</v>
+      </c>
       <c r="DI33" s="21"/>
       <c r="DJ33" s="24"/>
       <c r="DK33" s="7"/>
@@ -7679,11 +7775,11 @@
       <c r="EL33" s="22"/>
     </row>
     <row r="34" spans="1:142" ht="15" thickBot="1">
-      <c r="A34" s="86" t="s">
-        <v>35</v>
+      <c r="A34" s="93" t="s">
+        <v>32</v>
       </c>
       <c r="B34" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="21"/>
@@ -7843,9 +7939,9 @@
       <c r="EL34" s="22"/>
     </row>
     <row r="35" spans="1:142" ht="15" thickBot="1">
-      <c r="A35" s="87"/>
+      <c r="A35" s="94"/>
       <c r="B35" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35" s="20"/>
       <c r="D35" s="21"/>
@@ -7989,11 +8085,11 @@
       <c r="EL35" s="22"/>
     </row>
     <row r="36" spans="1:142" ht="15" thickBot="1">
-      <c r="A36" s="86" t="s">
-        <v>90</v>
+      <c r="A36" s="93" t="s">
+        <v>87</v>
       </c>
       <c r="B36" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36" s="20"/>
       <c r="D36" s="21"/>
@@ -8139,9 +8235,9 @@
       <c r="EL36" s="22"/>
     </row>
     <row r="37" spans="1:142" ht="15" thickBot="1">
-      <c r="A37" s="99"/>
+      <c r="A37" s="96"/>
       <c r="B37" s="66" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="31"/>
@@ -8286,6 +8382,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="X3:AD3"/>
+    <mergeCell ref="DY3:EE3"/>
+    <mergeCell ref="EF3:EL3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="DD3:DJ3"/>
+    <mergeCell ref="DK3:DQ3"/>
+    <mergeCell ref="DR5:DX5"/>
+    <mergeCell ref="DY5:EE5"/>
+    <mergeCell ref="EF5:EL5"/>
+    <mergeCell ref="BU5:CA5"/>
+    <mergeCell ref="CB5:CH5"/>
+    <mergeCell ref="CI5:CO5"/>
+    <mergeCell ref="CP5:CV5"/>
+    <mergeCell ref="CW5:DC5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="CB3:CH3"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="DR3:DX3"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="CI3:CO3"/>
+    <mergeCell ref="CP3:CV3"/>
+    <mergeCell ref="CW3:DC3"/>
+    <mergeCell ref="BU3:CA3"/>
+    <mergeCell ref="AE3:AK3"/>
+    <mergeCell ref="AL3:AR3"/>
+    <mergeCell ref="AS3:AY3"/>
+    <mergeCell ref="AZ3:BF3"/>
+    <mergeCell ref="BG3:BM3"/>
+    <mergeCell ref="BN3:BT3"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="DD5:DJ5"/>
@@ -8302,48 +8440,6 @@
     <mergeCell ref="AE5:AK5"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="DR3:DX3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="CI3:CO3"/>
-    <mergeCell ref="CP3:CV3"/>
-    <mergeCell ref="CW3:DC3"/>
-    <mergeCell ref="BU3:CA3"/>
-    <mergeCell ref="AE3:AK3"/>
-    <mergeCell ref="AL3:AR3"/>
-    <mergeCell ref="AS3:AY3"/>
-    <mergeCell ref="AZ3:BF3"/>
-    <mergeCell ref="BG3:BM3"/>
-    <mergeCell ref="BN3:BT3"/>
-    <mergeCell ref="DY3:EE3"/>
-    <mergeCell ref="EF3:EL3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="DD3:DJ3"/>
-    <mergeCell ref="DK3:DQ3"/>
-    <mergeCell ref="DR5:DX5"/>
-    <mergeCell ref="DY5:EE5"/>
-    <mergeCell ref="EF5:EL5"/>
-    <mergeCell ref="BU5:CA5"/>
-    <mergeCell ref="CB5:CH5"/>
-    <mergeCell ref="CI5:CO5"/>
-    <mergeCell ref="CP5:CV5"/>
-    <mergeCell ref="CW5:DC5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="CB3:CH3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="X3:AD3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8354,8 +8450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FF6EFD-F608-4DA6-AB00-E35874012156}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="109" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A10" zoomScale="109" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -8367,24 +8463,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="19">
       <c r="A1" s="109" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="109"/>
       <c r="C1" s="62"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="61" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="110" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="110"/>
       <c r="D3" s="60"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="61" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" s="112">
         <v>1</v>
@@ -8394,17 +8490,17 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="61" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="110" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" s="110"/>
       <c r="D5" s="60"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="61" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="113">
         <v>45524</v>
@@ -8414,7 +8510,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="61" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="114">
         <v>45671</v>
@@ -8424,10 +8520,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="61" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="110" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="110"/>
       <c r="D8" s="60"/>
@@ -8440,10 +8536,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="60" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="111" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C10" s="111"/>
       <c r="D10" s="111"/>
@@ -8463,7 +8559,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="111" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B13" s="111"/>
       <c r="C13" s="111"/>
@@ -8472,13 +8568,13 @@
     <row r="14" spans="1:5" ht="15" thickBot="1"/>
     <row r="15" spans="1:5" ht="15" thickBot="1">
       <c r="A15" s="74" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -8486,10 +8582,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -8497,10 +8593,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -8508,10 +8604,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -8519,10 +8615,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -8530,10 +8626,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -8541,10 +8637,10 @@
         <v>6</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -8552,10 +8648,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D22" s="60"/>
       <c r="E22" s="60"/>
@@ -8568,13 +8664,13 @@
         <v>8</v>
       </c>
       <c r="B23" s="55" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23" s="116" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E23" s="117"/>
       <c r="F23" s="117"/>
@@ -8586,10 +8682,10 @@
         <v>9</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D24" s="60"/>
       <c r="E24" s="60"/>
@@ -8602,10 +8698,10 @@
         <v>10</v>
       </c>
       <c r="B25" s="56" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
@@ -8618,10 +8714,10 @@
         <v>11</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
@@ -8634,10 +8730,10 @@
         <v>12</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D27" s="60"/>
       <c r="E27" s="60"/>
@@ -8650,10 +8746,10 @@
         <v>13</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D28" s="60"/>
       <c r="E28" s="60"/>
@@ -8666,13 +8762,13 @@
         <v>14</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D29" s="115" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E29" s="111"/>
       <c r="F29" s="60"/>
@@ -8684,10 +8780,10 @@
         <v>15</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
@@ -8700,10 +8796,10 @@
         <v>16</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D31" s="60"/>
       <c r="E31" s="60"/>
@@ -8716,10 +8812,10 @@
         <v>17</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D32" s="60"/>
       <c r="E32" s="60"/>
@@ -8732,10 +8828,10 @@
         <v>18</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -8744,7 +8840,7 @@
       </c>
       <c r="B34" s="38"/>
       <c r="C34" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -8753,7 +8849,7 @@
       </c>
       <c r="B35" s="37"/>
       <c r="C35" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -8762,7 +8858,7 @@
       </c>
       <c r="B36" s="38"/>
       <c r="C36" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -8771,7 +8867,7 @@
       </c>
       <c r="B37" s="37"/>
       <c r="C37" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" thickBot="1">
@@ -8781,7 +8877,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="111" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B42" s="111"/>
       <c r="C42" s="111"/>
@@ -8789,13 +8885,13 @@
     <row r="43" spans="1:3" ht="15" thickBot="1"/>
     <row r="44" spans="1:3" ht="15" thickBot="1">
       <c r="A44" s="74" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B44" s="75" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C44" s="75" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -8803,10 +8899,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="53" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -8814,10 +8910,10 @@
         <v>2</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -8825,10 +8921,10 @@
         <v>3</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -8836,10 +8932,10 @@
         <v>4</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -8847,10 +8943,10 @@
         <v>5</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -8858,10 +8954,10 @@
         <v>6</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -8869,10 +8965,10 @@
         <v>7</v>
       </c>
       <c r="B51" s="38" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -8880,10 +8976,10 @@
         <v>8</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C52" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -8891,10 +8987,10 @@
         <v>9</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -8902,10 +8998,10 @@
         <v>10</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -8914,7 +9010,7 @@
       </c>
       <c r="B55" s="38"/>
       <c r="C55" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15" thickBot="1">
@@ -8945,7 +9041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE61892C-FE6C-4A4A-BAF9-D966EA164C2A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData/>

</xml_diff>